<commit_message>
- code fix to honor fail-immediate on critical commands such as [web &raquo; `open(url)`](../commands/web/open(url)).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11068" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11537" uniqueCount="475">
   <si>
     <t>description</t>
   </si>
@@ -1497,7 +1497,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="356" x14ac:knownFonts="1">
+  <fonts count="371" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3736,8 +3736,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="625">
+  <fills count="652">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7275,8 +7369,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="647">
+  <borders count="675">
     <border>
       <left/>
       <right/>
@@ -13800,6 +14047,288 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -13807,7 +14336,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="383">
+  <cellXfs count="398">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -14930,49 +15459,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="340" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="341" fillId="600" borderId="626" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="626" fillId="600" fontId="341" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="342" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="342" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="343" fillId="603" borderId="630" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="630" fillId="603" fontId="343" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="344" fillId="606" borderId="634" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="634" fillId="606" fontId="344" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="345" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="345" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="346" fillId="609" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="609" fontId="346" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="347" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="347" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="348" fillId="612" borderId="638" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="638" fillId="612" fontId="348" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="349" fillId="615" borderId="642" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="642" fillId="615" fontId="349" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="350" fillId="618" borderId="646" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="646" fillId="618" fontId="350" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="351" fillId="618" borderId="646" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="646" fillId="618" fontId="351" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="352" fillId="621" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="621" fontId="352" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="353" fillId="624" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="624" fontId="353" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="354" fillId="621" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="621" fontId="354" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="355" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="355" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="356" fillId="627" borderId="654" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="357" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="358" fillId="630" borderId="658" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="359" fillId="633" borderId="662" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="360" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="361" fillId="636" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="362" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="363" fillId="639" borderId="666" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="364" fillId="642" borderId="670" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="365" fillId="645" borderId="674" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="366" fillId="645" borderId="674" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="367" fillId="648" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="368" fillId="651" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="369" fillId="648" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="370" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[xml] - [`append(xml,xpath,content,var)`]: **NEW** command to append content to an XML document - [`prepend(xml,xpath,content,var)`]: **NEW** command to prepend content to an XML document - [`clear(xml,xpath,var)`]: **NEW** command to clear content in an XML document - [`delete(xml,xpath,var)`]: **NEW** command to delete nodes from an XML document - [`replace(xml,xpath,content,var)`]: **NEW** command to replace content in an XML document
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
@@ -21,38 +21,39 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$D$2:$D$38</definedName>
-    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
+    <definedName name="base">'#system'!$E$2:$E$38</definedName>
+    <definedName name="csv">'#system'!$F$2:$F$5</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
-    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
-    <definedName name="external">'#system'!$H$2:$H$4</definedName>
-    <definedName name="image">'#system'!$I$2:$I$6</definedName>
-    <definedName name="io">'#system'!$J$2:$J$25</definedName>
-    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
-    <definedName name="json">'#system'!$L$2:$L$16</definedName>
-    <definedName name="mail">'#system'!$N$2:$N$2</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$92</definedName>
+    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
+    <definedName name="external">'#system'!$I$2:$I$4</definedName>
+    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="io">'#system'!$K$2:$K$25</definedName>
+    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
+    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="mail">'#system'!$O$2:$O$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$O$2:$O$15</definedName>
-    <definedName name="pdf">'#system'!$P$2:$P$16</definedName>
-    <definedName name="rdbms">'#system'!$Q$2:$Q$7</definedName>
-    <definedName name="redis">'#system'!$R$2:$R$10</definedName>
-    <definedName name="sms">'#system'!$S$2:$S$2</definedName>
-    <definedName name="sound">'#system'!$T$2:$T$5</definedName>
-    <definedName name="ssh">'#system'!$U$2:$U$9</definedName>
-    <definedName name="step">'#system'!$V$2:$V$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$28</definedName>
-    <definedName name="web">'#system'!$W$2:$W$122</definedName>
-    <definedName name="webalert">'#system'!$X$2:$X$8</definedName>
-    <definedName name="webcookie">'#system'!$Y$2:$Y$8</definedName>
-    <definedName name="ws">'#system'!$Z$2:$Z$17</definedName>
-    <definedName name="ws.async">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="xml">'#system'!$AB$2:$AB$13</definedName>
+    <definedName name="number">'#system'!$P$2:$P$15</definedName>
+    <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
+    <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
+    <definedName name="redis">'#system'!$S$2:$S$10</definedName>
+    <definedName name="sms">'#system'!$T$2:$T$2</definedName>
+    <definedName name="sound">'#system'!$U$2:$U$5</definedName>
+    <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
+    <definedName name="step">'#system'!$W$2:$W$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$29</definedName>
+    <definedName name="web">'#system'!$X$2:$X$122</definedName>
+    <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
+    <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
+    <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="xml">'#system'!$AC$2:$AC$18</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="macro">'#system'!$M$2:$M$4</definedName>
+    <definedName name="macro">'#system'!$N$2:$N$4</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17316" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18321" uniqueCount="513">
   <si>
     <t>description</t>
   </si>
@@ -1577,13 +1578,43 @@
   <si>
     <t>saveAttributeList(var,locator,attrName)</t>
   </si>
+  <si>
+    <t>aws.sqs</t>
+  </si>
+  <si>
+    <t>deleteMessage(profile,queue,receiptHandle)</t>
+  </si>
+  <si>
+    <t>receiveMessage(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>receiveMessages(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>sendMessage(profile,queue,message,var)</t>
+  </si>
+  <si>
+    <t>append(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>clear(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>delete(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>prepend(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replace(xml,xpath,content,var)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="563" x14ac:knownFonts="1">
+  <fonts count="595" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5128,8 +5159,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="976">
+  <fills count="1030">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10656,8 +10889,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1011">
+  <borders count="1067">
     <border>
       <left/>
       <right/>
@@ -20847,6 +21386,570 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -20854,7 +21957,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="590">
+  <cellXfs count="622">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -22595,52 +23698,148 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="546" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="547" fillId="951" borderId="990" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="990" fillId="951" fontId="547" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="548" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="548" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="549" fillId="954" borderId="994" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="994" fillId="954" fontId="549" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="550" fillId="957" borderId="998" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="998" fillId="957" fontId="550" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="551" fillId="960" borderId="998" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="998" fillId="960" fontId="551" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="552" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="552" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="553" fillId="963" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="963" fontId="553" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="554" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="554" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="555" fillId="966" borderId="1002" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1002" fillId="966" fontId="555" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="556" fillId="969" borderId="1006" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1006" fillId="969" fontId="556" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="557" fillId="972" borderId="1010" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1010" fillId="972" fontId="557" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="558" fillId="972" borderId="1010" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1010" fillId="972" fontId="558" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="559" fillId="960" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="960" fontId="559" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="560" fillId="975" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="975" fontId="560" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="561" fillId="960" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="960" fontId="561" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="562" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="562" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1018" fillId="978" fontId="563" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="564" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1022" fillId="981" fontId="565" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1026" fillId="984" fontId="566" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1026" fillId="987" fontId="567" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="568" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="990" fontId="569" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="570" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1030" fillId="993" fontId="571" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1034" fillId="996" fontId="572" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1038" fillId="999" fontId="573" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1038" fillId="999" fontId="574" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="987" fontId="575" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1002" fontId="576" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="987" fontId="577" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="578" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="579" fillId="1005" borderId="1046" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="580" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="581" fillId="1008" borderId="1050" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="582" fillId="1011" borderId="1054" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="583" fillId="1014" borderId="1054" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="584" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="585" fillId="1017" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="586" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="587" fillId="1020" borderId="1058" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="588" fillId="1023" borderId="1062" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="589" fillId="1026" borderId="1066" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="590" fillId="1026" borderId="1066" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="591" fillId="1014" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="592" fillId="1029" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="593" fillId="1014" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="594" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -23055,7 +24254,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC122"/>
+  <dimension ref="A1:AD122"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -23077,78 +24276,81 @@
         <v>475</v>
       </c>
       <c r="D1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>348</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>334</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>494</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>197</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>240</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>411</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>423</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>424</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>358</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>407</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>425</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>228</v>
       </c>
     </row>
@@ -23163,79 +24365,82 @@
         <v>480</v>
       </c>
       <c r="D2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>464</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>484</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>316</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>395</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>429</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>497</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>430</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>431</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>254</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>218</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>412</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>435</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>436</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>382</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>408</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>98</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>172</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>177</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>184</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>444</v>
       </c>
-      <c r="AB2" t="s">
-        <v>229</v>
+      <c r="AC2" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="3">
@@ -23249,1546 +24454,1573 @@
         <v>477</v>
       </c>
       <c r="D3" t="s">
+        <v>505</v>
+      </c>
+      <c r="E3" t="s">
         <v>472</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>366</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>89</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>495</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>350</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>342</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>335</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>87</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>498</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>432</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>241</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>219</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>413</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>437</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>383</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>409</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>99</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>173</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>178</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>365</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>185</v>
       </c>
-      <c r="AB3" t="s">
-        <v>230</v>
+      <c r="AC3" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>503</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
       </c>
       <c r="D4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>398</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>465</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>496</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>351</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>239</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>336</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>499</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>26</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>242</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>220</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>414</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>438</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>359</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>410</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>355</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>174</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>179</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>185</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>445</v>
       </c>
-      <c r="AB4" t="s">
-        <v>231</v>
+      <c r="AC4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
       </c>
       <c r="D5" t="s">
+        <v>507</v>
+      </c>
+      <c r="E5" t="s">
         <v>473</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>452</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>337</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>470</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>352</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>478</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>88</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>30</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>243</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>221</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>415</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>439</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>360</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>356</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>175</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>180</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>186</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>446</v>
       </c>
-      <c r="AB5" t="s">
-        <v>232</v>
+      <c r="AC5" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>399</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>462</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>349</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>73</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>29</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>31</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>244</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>402</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>416</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>362</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>100</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>458</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>181</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>187</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>447</v>
       </c>
-      <c r="AB6" t="s">
-        <v>233</v>
+      <c r="AC6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>225</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>367</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>461</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>16</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>316</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>33</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>245</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>434</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>417</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>361</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>101</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>459</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>182</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>188</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>448</v>
       </c>
-      <c r="AB7" t="s">
-        <v>234</v>
+      <c r="AC7" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>319</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>368</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>329</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>81</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>34</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>92</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>246</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>418</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>363</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>102</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>176</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>183</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>189</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>449</v>
       </c>
-      <c r="AB8" t="s">
-        <v>235</v>
+      <c r="AC8" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>307</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>330</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>38</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>93</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>247</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>419</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>364</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>210</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>190</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G10" t="s">
+        <v>353</v>
+      </c>
+      <c r="H10" t="s">
+        <v>466</v>
+      </c>
+      <c r="K10" t="s">
+        <v>401</v>
+      </c>
+      <c r="M10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>248</v>
+      </c>
+      <c r="S10" t="s">
+        <v>420</v>
+      </c>
+      <c r="X10" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC10" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="11">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>316</v>
+      <c r="E11" t="s">
+        <v>256</v>
       </c>
-      <c r="F10" t="s">
-        <v>353</v>
+      <c r="G11" t="s">
+        <v>275</v>
       </c>
-      <c r="G10" t="s">
-        <v>466</v>
+      <c r="H11" t="s">
+        <v>323</v>
       </c>
-      <c r="J10" t="s">
-        <v>401</v>
+      <c r="K11" t="s">
+        <v>17</v>
       </c>
-      <c r="L10" t="s">
-        <v>36</v>
+      <c r="M11" t="s">
+        <v>489</v>
       </c>
-      <c r="O10" t="s">
-        <v>433</v>
+      <c r="P11" t="s">
+        <v>94</v>
       </c>
-      <c r="P10" t="s">
-        <v>248</v>
+      <c r="Q11" t="s">
+        <v>249</v>
       </c>
-      <c r="R10" t="s">
-        <v>420</v>
+      <c r="X11" t="s">
+        <v>259</v>
       </c>
-      <c r="W10" t="s">
-        <v>258</v>
+      <c r="AA11" t="s">
+        <v>260</v>
       </c>
-      <c r="Z10" t="s">
-        <v>191</v>
+      <c r="AC11" t="s">
+        <v>509</v>
       </c>
-      <c r="AB10" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E12" t="s">
+        <v>320</v>
+      </c>
+      <c r="G12" t="s">
+        <v>264</v>
+      </c>
+      <c r="H12" t="s">
+        <v>324</v>
+      </c>
+      <c r="K12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>454</v>
+      </c>
+      <c r="P12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>250</v>
+      </c>
+      <c r="X12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>342</v>
+      </c>
+      <c r="G13" t="s">
+        <v>317</v>
+      </c>
+      <c r="H13" t="s">
+        <v>325</v>
+      </c>
+      <c r="K13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
+        <v>490</v>
+      </c>
+      <c r="P13" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>255</v>
+      </c>
+      <c r="X13" t="s">
+        <v>327</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC13" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>334</v>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>494</v>
       </c>
-      <c r="D11" t="s">
-        <v>256</v>
+      <c r="E14" t="s">
+        <v>37</v>
       </c>
-      <c r="F11" t="s">
-        <v>275</v>
+      <c r="G14" t="s">
+        <v>265</v>
       </c>
-      <c r="G11" t="s">
-        <v>323</v>
+      <c r="H14" t="s">
+        <v>326</v>
       </c>
-      <c r="J11" t="s">
-        <v>17</v>
+      <c r="K14" t="s">
+        <v>83</v>
       </c>
-      <c r="L11" t="s">
-        <v>489</v>
+      <c r="M14" t="s">
+        <v>39</v>
       </c>
-      <c r="O11" t="s">
-        <v>94</v>
+      <c r="P14" t="s">
+        <v>96</v>
       </c>
-      <c r="P11" t="s">
-        <v>249</v>
+      <c r="Q14" t="s">
+        <v>251</v>
       </c>
-      <c r="W11" t="s">
-        <v>259</v>
+      <c r="X14" t="s">
+        <v>104</v>
       </c>
-      <c r="Z11" t="s">
-        <v>260</v>
+      <c r="AA14" t="s">
+        <v>194</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC14" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>266</v>
+      </c>
+      <c r="K15" t="s">
+        <v>471</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>252</v>
+      </c>
+      <c r="X15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>396</v>
+      </c>
+      <c r="G16" t="s">
+        <v>318</v>
+      </c>
+      <c r="K16" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>253</v>
+      </c>
+      <c r="X16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC16" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>24</v>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>240</v>
       </c>
-      <c r="D12" t="s">
-        <v>320</v>
+      <c r="E17" t="s">
+        <v>397</v>
       </c>
-      <c r="F12" t="s">
-        <v>264</v>
+      <c r="G17" t="s">
+        <v>90</v>
       </c>
-      <c r="G12" t="s">
-        <v>324</v>
+      <c r="K17" t="s">
+        <v>85</v>
       </c>
-      <c r="J12" t="s">
-        <v>42</v>
+      <c r="X17" t="s">
+        <v>106</v>
       </c>
-      <c r="L12" t="s">
-        <v>454</v>
+      <c r="AA17" t="s">
+        <v>479</v>
       </c>
-      <c r="O12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P12" t="s">
-        <v>250</v>
-      </c>
-      <c r="W12" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB12" t="s">
+      <c r="AC17" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>494</v>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>342</v>
+      <c r="E18" t="s">
+        <v>426</v>
       </c>
-      <c r="F13" t="s">
-        <v>317</v>
+      <c r="G18" t="s">
+        <v>91</v>
       </c>
-      <c r="G13" t="s">
-        <v>325</v>
+      <c r="K18" t="s">
+        <v>381</v>
       </c>
-      <c r="J13" t="s">
-        <v>82</v>
+      <c r="X18" t="s">
+        <v>107</v>
       </c>
-      <c r="L13" t="s">
-        <v>490</v>
-      </c>
-      <c r="O13" t="s">
-        <v>95</v>
-      </c>
-      <c r="P13" t="s">
-        <v>255</v>
-      </c>
-      <c r="W13" t="s">
-        <v>327</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB13" t="s">
+      <c r="AC18" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
-        <v>265</v>
-      </c>
-      <c r="G14" t="s">
-        <v>326</v>
-      </c>
-      <c r="J14" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" t="s">
-        <v>96</v>
-      </c>
-      <c r="P14" t="s">
-        <v>251</v>
-      </c>
-      <c r="W14" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J15" t="s">
-        <v>471</v>
-      </c>
-      <c r="L15" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" t="s">
-        <v>97</v>
-      </c>
-      <c r="P15" t="s">
-        <v>252</v>
-      </c>
-      <c r="W15" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>240</v>
-      </c>
-      <c r="D16" t="s">
-        <v>396</v>
-      </c>
-      <c r="F16" t="s">
-        <v>318</v>
-      </c>
-      <c r="J16" t="s">
-        <v>84</v>
-      </c>
-      <c r="L16" t="s">
-        <v>43</v>
-      </c>
-      <c r="P16" t="s">
-        <v>253</v>
-      </c>
-      <c r="W16" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>397</v>
-      </c>
-      <c r="F17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" t="s">
-        <v>85</v>
-      </c>
-      <c r="W17" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="19">
+      <c r="A19" t="s">
         <v>411</v>
       </c>
-      <c r="D18" t="s">
-        <v>426</v>
+      <c r="E19" t="s">
+        <v>61</v>
       </c>
-      <c r="F18" t="s">
-        <v>91</v>
+      <c r="G19" t="s">
+        <v>297</v>
       </c>
-      <c r="J18" t="s">
-        <v>381</v>
+      <c r="K19" t="s">
+        <v>488</v>
       </c>
-      <c r="W18" t="s">
-        <v>107</v>
+      <c r="X19" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="20">
+      <c r="A20" t="s">
         <v>423</v>
       </c>
-      <c r="D19" t="s">
-        <v>61</v>
+      <c r="E20" t="s">
+        <v>62</v>
       </c>
-      <c r="F19" t="s">
-        <v>297</v>
+      <c r="G20" t="s">
+        <v>298</v>
       </c>
-      <c r="J19" t="s">
-        <v>488</v>
+      <c r="K20" t="s">
+        <v>44</v>
       </c>
-      <c r="W19" t="s">
-        <v>108</v>
+      <c r="X20" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="21">
+      <c r="A21" t="s">
         <v>424</v>
       </c>
-      <c r="D20" t="s">
-        <v>62</v>
+      <c r="E21" t="s">
+        <v>257</v>
       </c>
-      <c r="F20" t="s">
-        <v>298</v>
+      <c r="G21" t="s">
+        <v>299</v>
       </c>
-      <c r="J20" t="s">
-        <v>44</v>
+      <c r="K21" t="s">
+        <v>403</v>
       </c>
-      <c r="W20" t="s">
-        <v>109</v>
+      <c r="X21" t="s">
+        <v>500</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>358</v>
       </c>
-      <c r="D21" t="s">
-        <v>257</v>
+      <c r="E22" t="s">
+        <v>63</v>
       </c>
-      <c r="F21" t="s">
-        <v>299</v>
+      <c r="G22" t="s">
+        <v>300</v>
       </c>
-      <c r="J21" t="s">
-        <v>403</v>
+      <c r="K22" t="s">
+        <v>86</v>
       </c>
-      <c r="W21" t="s">
-        <v>500</v>
+      <c r="X22" t="s">
+        <v>111</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="23">
+      <c r="A23" t="s">
         <v>407</v>
       </c>
-      <c r="D22" t="s">
-        <v>63</v>
+      <c r="E23" t="s">
+        <v>322</v>
       </c>
-      <c r="F22" t="s">
-        <v>300</v>
+      <c r="G23" t="s">
+        <v>291</v>
       </c>
-      <c r="J22" t="s">
-        <v>86</v>
+      <c r="K23" t="s">
+        <v>453</v>
       </c>
-      <c r="W22" t="s">
-        <v>111</v>
+      <c r="X23" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="24">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
-      <c r="D23" t="s">
-        <v>322</v>
+      <c r="E24" t="s">
+        <v>64</v>
       </c>
-      <c r="F23" t="s">
-        <v>291</v>
+      <c r="G24" t="s">
+        <v>280</v>
       </c>
-      <c r="J23" t="s">
-        <v>453</v>
+      <c r="K24" t="s">
+        <v>45</v>
       </c>
-      <c r="W23" t="s">
-        <v>112</v>
+      <c r="X24" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="25">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="D24" t="s">
-        <v>64</v>
+      <c r="E25" t="s">
+        <v>463</v>
       </c>
-      <c r="F24" t="s">
-        <v>280</v>
+      <c r="G25" t="s">
+        <v>77</v>
       </c>
-      <c r="J24" t="s">
-        <v>45</v>
+      <c r="K25" t="s">
+        <v>46</v>
       </c>
-      <c r="W24" t="s">
-        <v>113</v>
+      <c r="X25" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="26">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
-        <v>463</v>
+      <c r="E26" t="s">
+        <v>226</v>
       </c>
-      <c r="F25" t="s">
-        <v>77</v>
+      <c r="G26" t="s">
+        <v>283</v>
       </c>
-      <c r="J25" t="s">
-        <v>46</v>
+      <c r="X26" t="s">
+        <v>115</v>
       </c>
-      <c r="W25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="D26" t="s">
-        <v>226</v>
+      <c r="E27" t="s">
+        <v>227</v>
       </c>
-      <c r="F26" t="s">
-        <v>283</v>
+      <c r="G27" t="s">
+        <v>267</v>
       </c>
-      <c r="W26" t="s">
-        <v>115</v>
+      <c r="X27" t="s">
+        <v>328</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="28">
+      <c r="A28" t="s">
         <v>425</v>
       </c>
-      <c r="D27" t="s">
-        <v>227</v>
+      <c r="E28" t="s">
+        <v>486</v>
       </c>
-      <c r="F27" t="s">
-        <v>267</v>
+      <c r="G28" t="s">
+        <v>284</v>
       </c>
-      <c r="W27" t="s">
-        <v>328</v>
+      <c r="X28" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s">
+    <row r="29">
+      <c r="A29" t="s">
         <v>228</v>
       </c>
-      <c r="D28" t="s">
-        <v>486</v>
-      </c>
-      <c r="F28" t="s">
-        <v>284</v>
-      </c>
-      <c r="W28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>487</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>285</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="30">
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>427</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>217</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="31">
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>65</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>276</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="32">
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>66</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>286</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="33">
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>67</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>261</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="34">
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>68</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>331</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="35">
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>69</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>308</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="36">
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>70</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>262</v>
       </c>
-      <c r="W36" t="s">
+      <c r="X36" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="37">
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>71</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>309</v>
       </c>
-      <c r="W37" t="s">
+      <c r="X37" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="38">
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>72</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>268</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="39">
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>79</v>
       </c>
-      <c r="W39" t="s">
+      <c r="X39" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="40">
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>213</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="41">
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>290</v>
       </c>
-      <c r="W41" t="s">
+      <c r="X41" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="42">
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>301</v>
       </c>
-      <c r="W42" t="s">
+      <c r="X42" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="43">
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>302</v>
       </c>
-      <c r="W43" t="s">
+      <c r="X43" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="44">
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>344</v>
       </c>
-      <c r="W44" t="s">
+      <c r="X44" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="45">
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>343</v>
       </c>
-      <c r="W45" t="s">
+      <c r="X45" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="46">
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>212</v>
       </c>
-      <c r="W46" t="s">
+      <c r="X46" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="47">
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>321</v>
       </c>
-      <c r="W47" t="s">
+      <c r="X47" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="48">
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>340</v>
       </c>
-      <c r="W48" t="s">
+      <c r="X48" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="49">
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>369</v>
       </c>
-      <c r="W49" t="s">
+      <c r="X49" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="50">
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>303</v>
       </c>
-      <c r="W50" t="s">
+      <c r="X50" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="51">
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>357</v>
       </c>
-      <c r="W51" t="s">
+      <c r="X51" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="52">
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>332</v>
       </c>
-      <c r="W52" t="s">
+      <c r="X52" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="53">
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>269</v>
       </c>
-      <c r="W53" t="s">
+      <c r="X53" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="54">
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>293</v>
       </c>
-      <c r="W54" t="s">
+      <c r="X54" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="55">
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>294</v>
       </c>
-      <c r="W55" t="s">
+      <c r="X55" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="56">
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>295</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="57">
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>304</v>
       </c>
-      <c r="W57" t="s">
+      <c r="X57" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="58">
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>313</v>
       </c>
-      <c r="W58" t="s">
+      <c r="X58" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="59">
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>338</v>
       </c>
-      <c r="W59" t="s">
+      <c r="X59" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="60">
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>310</v>
       </c>
-      <c r="W60" t="s">
+      <c r="X60" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="61">
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>311</v>
       </c>
-      <c r="W61" t="s">
+      <c r="X61" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="62">
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>370</v>
       </c>
-      <c r="W62" t="s">
+      <c r="X62" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="63">
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>371</v>
       </c>
-      <c r="W63" t="s">
+      <c r="X63" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="64">
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>346</v>
       </c>
-      <c r="W64" t="s">
+      <c r="X64" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="65">
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>314</v>
       </c>
-      <c r="W65" t="s">
+      <c r="X65" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="66">
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>270</v>
       </c>
-      <c r="W66" t="s">
+      <c r="X66" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="67">
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>354</v>
       </c>
-      <c r="W67" t="s">
+      <c r="X67" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="68">
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>315</v>
       </c>
-      <c r="W68" t="s">
+      <c r="X68" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="69">
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>421</v>
       </c>
-      <c r="W69" t="s">
+      <c r="X69" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="70">
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>305</v>
       </c>
-      <c r="W70" t="s">
+      <c r="X70" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="71">
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>422</v>
       </c>
-      <c r="W71" t="s">
+      <c r="X71" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="72">
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>263</v>
       </c>
-      <c r="W72" t="s">
+      <c r="X72" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="73">
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>345</v>
       </c>
-      <c r="W73" t="s">
+      <c r="X73" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="74">
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>281</v>
       </c>
-      <c r="W74" t="s">
+      <c r="X74" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="75">
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>287</v>
       </c>
-      <c r="W75" t="s">
+      <c r="X75" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="76">
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>292</v>
       </c>
-      <c r="W76" t="s">
+      <c r="X76" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="77">
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>428</v>
       </c>
-      <c r="W77" t="s">
+      <c r="X77" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="78">
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>333</v>
       </c>
-      <c r="W78" t="s">
+      <c r="X78" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="79">
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>271</v>
       </c>
-      <c r="W79" t="s">
+      <c r="X79" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="80">
-      <c r="F80" t="s">
+      <c r="G80" t="s">
         <v>282</v>
       </c>
-      <c r="W80" t="s">
+      <c r="X80" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="81">
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>288</v>
       </c>
-      <c r="W81" t="s">
+      <c r="X81" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="82">
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>277</v>
       </c>
-      <c r="W82" t="s">
+      <c r="X82" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="83">
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>272</v>
       </c>
-      <c r="W83" t="s">
+      <c r="X83" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="84">
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>289</v>
       </c>
-      <c r="W84" t="s">
+      <c r="X84" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="85">
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>273</v>
       </c>
-      <c r="W85" t="s">
+      <c r="X85" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="86">
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>274</v>
       </c>
-      <c r="W86" t="s">
+      <c r="X86" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="87">
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>306</v>
       </c>
-      <c r="W87" t="s">
+      <c r="X87" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="88">
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>312</v>
       </c>
-      <c r="W88" t="s">
+      <c r="X88" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="89">
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>296</v>
       </c>
-      <c r="W89" t="s">
+      <c r="X89" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="90">
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>341</v>
       </c>
-      <c r="W90" t="s">
+      <c r="X90" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="91">
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>278</v>
       </c>
-      <c r="W91" t="s">
+      <c r="X91" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="92">
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>279</v>
       </c>
-      <c r="W92" t="s">
+      <c r="X92" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="93">
-      <c r="W93" t="s">
+      <c r="X93" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="94">
-      <c r="W94" t="s">
+      <c r="X94" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="95">
-      <c r="W95" t="s">
+      <c r="X95" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="96">
-      <c r="W96" t="s">
+      <c r="X96" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="97">
-      <c r="W97" t="s">
+      <c r="X97" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="98">
-      <c r="W98" t="s">
+      <c r="X98" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="99">
-      <c r="W99" t="s">
+      <c r="X99" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="100">
-      <c r="W100" t="s">
+      <c r="X100" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="101">
-      <c r="W101" t="s">
+      <c r="X101" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="102">
-      <c r="W102" t="s">
+      <c r="X102" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="103">
-      <c r="W103" t="s">
+      <c r="X103" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="104">
-      <c r="W104" t="s">
+      <c r="X104" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="105">
-      <c r="W105" t="s">
+      <c r="X105" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="106">
-      <c r="W106" t="s">
+      <c r="X106" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="107">
-      <c r="W107" t="s">
+      <c r="X107" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="108">
-      <c r="W108" t="s">
+      <c r="X108" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="109">
-      <c r="W109" t="s">
+      <c r="X109" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="110">
-      <c r="W110" t="s">
+      <c r="X110" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="111">
-      <c r="W111" t="s">
+      <c r="X111" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="112">
-      <c r="W112" t="s">
+      <c r="X112" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="113">
-      <c r="W113" t="s">
+      <c r="X113" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="114">
-      <c r="W114" t="s">
+      <c r="X114" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="115">
-      <c r="W115" t="s">
+      <c r="X115" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="116">
-      <c r="W116" t="s">
+      <c r="X116" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="117">
-      <c r="W117" t="s">
+      <c r="X117" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="118">
-      <c r="W118" t="s">
+      <c r="X118" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="119">
-      <c r="W119" t="s">
+      <c r="X119" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="120">
-      <c r="W120" t="s">
+      <c r="X120" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="121">
-      <c r="W121" t="s">
+      <c r="X121" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="122">
-      <c r="W122" t="s">
+      <c r="X122" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[image commands] - [`ocr(source,saveVar)`]: performance improvement to cache OCR text for repeated use
[io commands]
- [`checksum(var,file)`]: **NEW** command to determine a file's checksum value.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
@@ -32,12 +32,12 @@
     <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
-    <definedName name="io">'#system'!$L$2:$L$31</definedName>
+    <definedName name="io">'#system'!$L$2:$L$32</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
-    <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
+    <definedName name="mail">'#system'!$Q$2:$Q$4</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3793" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5003" uniqueCount="642">
   <si>
     <t>description</t>
   </si>
@@ -1987,6 +1987,18 @@
   </si>
   <si>
     <t>openFile(filePath)</t>
+  </si>
+  <si>
+    <t>checksum(var,file)</t>
+  </si>
+  <si>
+    <t>clearMail(var)</t>
+  </si>
+  <si>
+    <t>composeMail(var,action,value)</t>
+  </si>
+  <si>
+    <t>send(profile,var)</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2006,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="96" x14ac:knownFonts="1">
+  <fonts count="130" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2606,8 +2618,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="124">
+  <fills count="172">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2624,6 +2850,278 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -3352,7 +3850,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="157">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3689,55 +4187,157 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="96" fontId="78" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="102" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="102" fontId="79" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="80" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="105" fontId="81" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="108" fontId="82" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="111" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="111" fontId="83" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="84" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="114" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="114" fontId="85" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="86" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="87" fillId="117" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="117" fontId="87" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="88" fillId="120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="120" fontId="88" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="89" fillId="108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="108" fontId="89" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="90" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="91" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="92" fillId="111" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="111" fontId="92" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="123" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="123" fontId="93" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="94" fillId="111" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="111" fontId="94" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="120" fontId="95" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="126" fontId="96" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="97" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="129" fontId="98" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="132" fontId="99" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="135" fontId="100" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="101" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="138" fontId="102" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="103" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="141" fontId="104" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="144" fontId="105" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="132" fontId="106" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="107" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="108" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="135" fontId="109" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="147" fontId="110" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="135" fontId="111" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="144" fontId="112" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="150" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="153" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="156" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="159" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="162" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="165" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="168" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="156" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="159" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="171" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="159" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="168" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4311,7 +4911,7 @@
         <v>480</v>
       </c>
       <c r="Q2" t="s">
-        <v>422</v>
+        <v>639</v>
       </c>
       <c r="R2" t="s">
         <v>423</v>
@@ -4405,6 +5005,9 @@
       <c r="P3" t="s">
         <v>481</v>
       </c>
+      <c r="Q3" t="s">
+        <v>640</v>
+      </c>
       <c r="R3" t="s">
         <v>424</v>
       </c>
@@ -4491,6 +5094,9 @@
       <c r="P4" t="s">
         <v>482</v>
       </c>
+      <c r="Q4" t="s">
+        <v>641</v>
+      </c>
       <c r="R4" t="s">
         <v>26</v>
       </c>
@@ -4702,7 +5308,7 @@
         <v>345</v>
       </c>
       <c r="L7" t="s">
-        <v>72</v>
+        <v>638</v>
       </c>
       <c r="N7" t="s">
         <v>312</v>
@@ -4764,7 +5370,7 @@
         <v>529</v>
       </c>
       <c r="L8" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="N8" t="s">
         <v>33</v>
@@ -4823,7 +5429,7 @@
         <v>326</v>
       </c>
       <c r="L9" t="s">
-        <v>504</v>
+        <v>16</v>
       </c>
       <c r="N9" t="s">
         <v>34</v>
@@ -4873,7 +5479,7 @@
         <v>570</v>
       </c>
       <c r="L10" t="s">
-        <v>80</v>
+        <v>504</v>
       </c>
       <c r="N10" t="s">
         <v>35</v>
@@ -4917,7 +5523,7 @@
         <v>571</v>
       </c>
       <c r="L11" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="N11" t="s">
         <v>472</v>
@@ -4955,7 +5561,7 @@
         <v>453</v>
       </c>
       <c r="L12" t="s">
-        <v>505</v>
+        <v>37</v>
       </c>
       <c r="N12" t="s">
         <v>530</v>
@@ -4993,7 +5599,7 @@
         <v>319</v>
       </c>
       <c r="L13" t="s">
-        <v>393</v>
+        <v>505</v>
       </c>
       <c r="N13" t="s">
         <v>444</v>
@@ -5031,7 +5637,7 @@
         <v>320</v>
       </c>
       <c r="L14" t="s">
-        <v>17</v>
+        <v>393</v>
       </c>
       <c r="N14" t="s">
         <v>473</v>
@@ -5066,7 +5672,7 @@
         <v>321</v>
       </c>
       <c r="L15" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="N15" t="s">
         <v>38</v>
@@ -5101,7 +5707,7 @@
         <v>322</v>
       </c>
       <c r="L16" t="s">
-        <v>506</v>
+        <v>41</v>
       </c>
       <c r="N16" t="s">
         <v>541</v>
@@ -5133,7 +5739,7 @@
         <v>314</v>
       </c>
       <c r="L17" t="s">
-        <v>81</v>
+        <v>506</v>
       </c>
       <c r="N17" t="s">
         <v>39</v>
@@ -5162,7 +5768,7 @@
         <v>89</v>
       </c>
       <c r="L18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N18" t="s">
         <v>42</v>
@@ -5188,7 +5794,7 @@
         <v>90</v>
       </c>
       <c r="L19" t="s">
-        <v>457</v>
+        <v>82</v>
       </c>
       <c r="AA19" t="s">
         <v>502</v>
@@ -5208,7 +5814,7 @@
         <v>293</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>457</v>
       </c>
       <c r="AA20" t="s">
         <v>104</v>
@@ -5228,7 +5834,7 @@
         <v>294</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA21" t="s">
         <v>105</v>
@@ -5248,7 +5854,7 @@
         <v>295</v>
       </c>
       <c r="L22" t="s">
-        <v>554</v>
+        <v>84</v>
       </c>
       <c r="AA22" t="s">
         <v>106</v>
@@ -5268,7 +5874,7 @@
         <v>296</v>
       </c>
       <c r="L23" t="s">
-        <v>471</v>
+        <v>554</v>
       </c>
       <c r="AA23" t="s">
         <v>107</v>
@@ -5288,7 +5894,7 @@
         <v>287</v>
       </c>
       <c r="L24" t="s">
-        <v>43</v>
+        <v>471</v>
       </c>
       <c r="AA24" t="s">
         <v>483</v>
@@ -5308,7 +5914,7 @@
         <v>276</v>
       </c>
       <c r="L25" t="s">
-        <v>395</v>
+        <v>43</v>
       </c>
       <c r="AA25" t="s">
         <v>108</v>
@@ -5328,7 +5934,7 @@
         <v>76</v>
       </c>
       <c r="L26" t="s">
-        <v>589</v>
+        <v>395</v>
       </c>
       <c r="AA26" t="s">
         <v>542</v>
@@ -5348,7 +5954,7 @@
         <v>279</v>
       </c>
       <c r="L27" t="s">
-        <v>523</v>
+        <v>589</v>
       </c>
       <c r="AA27" t="s">
         <v>109</v>
@@ -5368,7 +5974,7 @@
         <v>263</v>
       </c>
       <c r="L28" t="s">
-        <v>85</v>
+        <v>523</v>
       </c>
       <c r="AA28" t="s">
         <v>110</v>
@@ -5385,7 +5991,7 @@
         <v>280</v>
       </c>
       <c r="L29" t="s">
-        <v>443</v>
+        <v>85</v>
       </c>
       <c r="AA29" t="s">
         <v>111</v>
@@ -5402,7 +6008,7 @@
         <v>281</v>
       </c>
       <c r="L30" t="s">
-        <v>44</v>
+        <v>443</v>
       </c>
       <c r="AA30" t="s">
         <v>112</v>
@@ -5419,7 +6025,7 @@
         <v>214</v>
       </c>
       <c r="L31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA31" t="s">
         <v>324</v>
@@ -5434,6 +6040,9 @@
       </c>
       <c r="H32" t="s">
         <v>272</v>
+      </c>
+      <c r="L32" t="s">
+        <v>45</v>
       </c>
       <c r="AA32" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
[webmail] - improved extraction of "clickable" links on mailinator mails.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
@@ -24,12 +24,12 @@
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
-    <definedName name="base">'#system'!$F$2:$F$45</definedName>
+    <definedName name="base">'#system'!$F$2:$F$47</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$16</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$111</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$18</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$32</definedName>
@@ -50,15 +50,17 @@
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="step.inTime">'#system'!$Z$2:$Z$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$32</definedName>
+    <definedName name="target">'#system'!$A$2:$A$34</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
     <definedName name="tn.5250">'#system'!$AA$2:$AA$38</definedName>
-    <definedName name="web">'#system'!$AA$2:$AA$151</definedName>
+    <definedName name="web">'#system'!$AA$2:$AA$153</definedName>
     <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
-    <definedName name="ws">'#system'!$AD$2:$AD$17</definedName>
-    <definedName name="ws.async">'#system'!$AE$2:$AE$8</definedName>
-    <definedName name="xml">'#system'!$AF$2:$AF$27</definedName>
+    <definedName name="ws">'#system'!$AF$2:$AF$17</definedName>
+    <definedName name="ws.async">'#system'!$AG$2:$AG$8</definedName>
+    <definedName name="xml">'#system'!$AH$2:$AH$27</definedName>
+    <definedName name="webmail">'#system'!$AD$2:$AD$4</definedName>
+    <definedName name="word">'#system'!$AE$2:$AE$9</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -73,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5612" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6255" uniqueCount="685">
   <si>
     <t>description</t>
   </si>
@@ -2017,6 +2019,117 @@
   </si>
   <si>
     <t>split(pdf,saveTo)</t>
+  </si>
+  <si>
+    <t>webmail</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>assertVarsNotPresent(vars)</t>
+  </si>
+  <si>
+    <t>assertVarsPresent(vars)</t>
+  </si>
+  <si>
+    <t>check(name)</t>
+  </si>
+  <si>
+    <t>checkByLocator(locator)</t>
+  </si>
+  <si>
+    <t>clickMenuByLocator(locator,menu)</t>
+  </si>
+  <si>
+    <t>contextMenu(name,menu,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>contextMenuByLocator(locator,menu,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>doubleClick(name)</t>
+  </si>
+  <si>
+    <t>doubleClickByLocator(locator)</t>
+  </si>
+  <si>
+    <t>rightClickElementOffset(name,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>rightClickOffset(locator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>saveAllTableRows(var,csv)</t>
+  </si>
+  <si>
+    <t>saveComboOptions(var,name)</t>
+  </si>
+  <si>
+    <t>saveComboOptionsByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>saveTableRows(var,contains,csv)</t>
+  </si>
+  <si>
+    <t>saveTableRowsRange(var,beginRow,endRow,csv)</t>
+  </si>
+  <si>
+    <t>screenshot(name,file)</t>
+  </si>
+  <si>
+    <t>screenshotByLocator(locator,file)</t>
+  </si>
+  <si>
+    <t>uncheck(name)</t>
+  </si>
+  <si>
+    <t>uncheckByLocator(locator)</t>
+  </si>
+  <si>
+    <t>renameSheet(file,worksheet,newName)</t>
+  </si>
+  <si>
+    <t>xls2xlsx(xlsFile,xlsxFile)</t>
+  </si>
+  <si>
+    <t>assertLocation(search)</t>
+  </si>
+  <si>
+    <t>openInTab(name,url)</t>
+  </si>
+  <si>
+    <t>delete(profile,id)</t>
+  </si>
+  <si>
+    <t>read(var,profile,id)</t>
+  </si>
+  <si>
+    <t>search(var,profile,searchCriteria,duration)</t>
+  </si>
+  <si>
+    <t>assertContains(file,text)</t>
+  </si>
+  <si>
+    <t>assertNotContain(file,text)</t>
+  </si>
+  <si>
+    <t>assertNotReadOnly(file)</t>
+  </si>
+  <si>
+    <t>assertPassword(file,password)</t>
+  </si>
+  <si>
+    <t>assertReadOnly(file)</t>
+  </si>
+  <si>
+    <t>extractText(var,file)</t>
+  </si>
+  <si>
+    <t>readOnly(file,password)</t>
+  </si>
+  <si>
+    <t>removeProtection(file)</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="147" x14ac:knownFonts="1">
+  <fonts count="164" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2957,8 +3070,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="196">
+  <fills count="220">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2975,6 +3195,142 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -4111,7 +4467,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="191">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4650,6 +5006,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="146" fillId="192" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="198" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="201" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="204" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="210" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="213" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="216" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="204" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="219" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="162" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="216" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5064,7 +5471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG151"/>
+  <dimension ref="A1:AI153"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -5164,12 +5571,18 @@
         <v>56</v>
       </c>
       <c r="AD1" t="s">
+        <v>648</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>649</v>
+      </c>
+      <c r="AF1" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>417</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5262,12 +5675,18 @@
         <v>174</v>
       </c>
       <c r="AD2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AF2" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>434</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>491</v>
       </c>
     </row>
@@ -5354,12 +5773,18 @@
         <v>175</v>
       </c>
       <c r="AD3" t="s">
+        <v>675</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>678</v>
+      </c>
+      <c r="AF3" t="s">
         <v>358</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>182</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5443,12 +5868,18 @@
         <v>176</v>
       </c>
       <c r="AD4" t="s">
+        <v>676</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AF4" t="s">
         <v>182</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>435</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>227</v>
       </c>
     </row>
@@ -5519,13 +5950,16 @@
       <c r="AC5" t="s">
         <v>568</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
+        <v>680</v>
+      </c>
+      <c r="AF5" t="s">
         <v>183</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>436</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5590,13 +6024,16 @@
       <c r="AC6" t="s">
         <v>177</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
+        <v>681</v>
+      </c>
+      <c r="AF6" t="s">
         <v>184</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>437</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5655,13 +6092,16 @@
       <c r="AC7" t="s">
         <v>178</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
+        <v>682</v>
+      </c>
+      <c r="AF7" t="s">
         <v>185</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>438</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>532</v>
       </c>
     </row>
@@ -5679,7 +6119,7 @@
         <v>360</v>
       </c>
       <c r="I8" t="s">
-        <v>325</v>
+        <v>670</v>
       </c>
       <c r="K8" t="s">
         <v>529</v>
@@ -5717,13 +6157,16 @@
       <c r="AC8" t="s">
         <v>179</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
+        <v>683</v>
+      </c>
+      <c r="AF8" t="s">
         <v>186</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>439</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>533</v>
       </c>
     </row>
@@ -5741,7 +6184,7 @@
         <v>361</v>
       </c>
       <c r="I9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L9" t="s">
         <v>16</v>
@@ -5773,10 +6216,13 @@
       <c r="AC9" t="s">
         <v>180</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
+        <v>684</v>
+      </c>
+      <c r="AF9" t="s">
         <v>187</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>534</v>
       </c>
     </row>
@@ -5791,7 +6237,7 @@
         <v>303</v>
       </c>
       <c r="I10" t="s">
-        <v>570</v>
+        <v>326</v>
       </c>
       <c r="L10" t="s">
         <v>504</v>
@@ -5817,10 +6263,10 @@
       <c r="AC10" t="s">
         <v>569</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AF10" t="s">
         <v>188</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5835,7 +6281,7 @@
         <v>349</v>
       </c>
       <c r="I11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L11" t="s">
         <v>80</v>
@@ -5855,10 +6301,10 @@
       <c r="AA11" t="s">
         <v>255</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AF11" t="s">
         <v>256</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>231</v>
       </c>
     </row>
@@ -5873,7 +6319,7 @@
         <v>271</v>
       </c>
       <c r="I12" t="s">
-        <v>453</v>
+        <v>571</v>
       </c>
       <c r="L12" t="s">
         <v>37</v>
@@ -5893,10 +6339,10 @@
       <c r="AA12" t="s">
         <v>101</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AF12" t="s">
         <v>189</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5911,7 +6357,7 @@
         <v>260</v>
       </c>
       <c r="I13" t="s">
-        <v>319</v>
+        <v>453</v>
       </c>
       <c r="L13" t="s">
         <v>505</v>
@@ -5931,10 +6377,10 @@
       <c r="AA13" t="s">
         <v>323</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AF13" t="s">
         <v>190</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5949,7 +6395,7 @@
         <v>313</v>
       </c>
       <c r="I14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L14" t="s">
         <v>393</v>
@@ -5966,10 +6412,10 @@
       <c r="AA14" t="s">
         <v>102</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AF14" t="s">
         <v>191</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>492</v>
       </c>
     </row>
@@ -5984,7 +6430,7 @@
         <v>261</v>
       </c>
       <c r="I15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L15" t="s">
         <v>17</v>
@@ -6001,10 +6447,10 @@
       <c r="AA15" t="s">
         <v>580</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AF15" t="s">
         <v>192</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>493</v>
       </c>
     </row>
@@ -6019,7 +6465,7 @@
         <v>262</v>
       </c>
       <c r="I16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L16" t="s">
         <v>41</v>
@@ -6036,10 +6482,10 @@
       <c r="AA16" t="s">
         <v>562</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AF16" t="s">
         <v>193</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>497</v>
       </c>
     </row>
@@ -6053,6 +6499,9 @@
       <c r="H17" t="s">
         <v>314</v>
       </c>
+      <c r="I17" t="s">
+        <v>322</v>
+      </c>
       <c r="L17" t="s">
         <v>506</v>
       </c>
@@ -6065,10 +6514,10 @@
       <c r="AA17" t="s">
         <v>103</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AF17" t="s">
         <v>464</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AH17" t="s">
         <v>498</v>
       </c>
     </row>
@@ -6082,6 +6531,9 @@
       <c r="H18" t="s">
         <v>89</v>
       </c>
+      <c r="I18" t="s">
+        <v>671</v>
+      </c>
       <c r="L18" t="s">
         <v>81</v>
       </c>
@@ -6094,7 +6546,7 @@
       <c r="AA18" t="s">
         <v>75</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AH18" t="s">
         <v>476</v>
       </c>
     </row>
@@ -6103,7 +6555,7 @@
         <v>237</v>
       </c>
       <c r="F19" t="s">
-        <v>418</v>
+        <v>650</v>
       </c>
       <c r="H19" t="s">
         <v>90</v>
@@ -6117,7 +6569,7 @@
       <c r="AA19" t="s">
         <v>502</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AH19" t="s">
         <v>494</v>
       </c>
     </row>
@@ -6126,7 +6578,7 @@
         <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>584</v>
+        <v>651</v>
       </c>
       <c r="H20" t="s">
         <v>293</v>
@@ -6140,7 +6592,7 @@
       <c r="AA20" t="s">
         <v>104</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AH20" t="s">
         <v>495</v>
       </c>
     </row>
@@ -6149,7 +6601,7 @@
         <v>403</v>
       </c>
       <c r="F21" t="s">
-        <v>585</v>
+        <v>418</v>
       </c>
       <c r="H21" t="s">
         <v>294</v>
@@ -6163,7 +6615,7 @@
       <c r="AA21" t="s">
         <v>105</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AH21" t="s">
         <v>499</v>
       </c>
     </row>
@@ -6172,7 +6624,7 @@
         <v>415</v>
       </c>
       <c r="F22" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H22" t="s">
         <v>295</v>
@@ -6183,7 +6635,7 @@
       <c r="AA22" t="s">
         <v>106</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AH22" t="s">
         <v>233</v>
       </c>
     </row>
@@ -6192,7 +6644,7 @@
         <v>416</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>585</v>
       </c>
       <c r="H23" t="s">
         <v>296</v>
@@ -6203,7 +6655,7 @@
       <c r="AA23" t="s">
         <v>107</v>
       </c>
-      <c r="AF23" t="s">
+      <c r="AH23" t="s">
         <v>535</v>
       </c>
     </row>
@@ -6212,7 +6664,7 @@
         <v>351</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>586</v>
       </c>
       <c r="H24" t="s">
         <v>287</v>
@@ -6223,7 +6675,7 @@
       <c r="AA24" t="s">
         <v>483</v>
       </c>
-      <c r="AF24" t="s">
+      <c r="AH24" t="s">
         <v>536</v>
       </c>
     </row>
@@ -6232,7 +6684,7 @@
         <v>399</v>
       </c>
       <c r="F25" t="s">
-        <v>253</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
         <v>276</v>
@@ -6243,7 +6695,7 @@
       <c r="AA25" t="s">
         <v>108</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AH25" t="s">
         <v>537</v>
       </c>
     </row>
@@ -6252,18 +6704,18 @@
         <v>573</v>
       </c>
       <c r="F26" t="s">
-        <v>587</v>
+        <v>61</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>652</v>
       </c>
       <c r="L26" t="s">
         <v>395</v>
       </c>
       <c r="AA26" t="s">
-        <v>542</v>
-      </c>
-      <c r="AF26" t="s">
+        <v>672</v>
+      </c>
+      <c r="AH26" t="s">
         <v>234</v>
       </c>
     </row>
@@ -6272,18 +6724,18 @@
         <v>54</v>
       </c>
       <c r="F27" t="s">
-        <v>538</v>
+        <v>253</v>
       </c>
       <c r="H27" t="s">
-        <v>279</v>
+        <v>653</v>
       </c>
       <c r="L27" t="s">
         <v>589</v>
       </c>
       <c r="AA27" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF27" t="s">
+        <v>542</v>
+      </c>
+      <c r="AH27" t="s">
         <v>235</v>
       </c>
     </row>
@@ -6292,16 +6744,16 @@
         <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>587</v>
       </c>
       <c r="H28" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="L28" t="s">
         <v>523</v>
       </c>
       <c r="AA28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
@@ -6309,898 +6761,959 @@
         <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>318</v>
+        <v>538</v>
       </c>
       <c r="H29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L29" t="s">
         <v>85</v>
       </c>
       <c r="AA29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>648</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="L30" t="s">
         <v>443</v>
       </c>
       <c r="AA30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>417</v>
+        <v>649</v>
       </c>
       <c r="F31" t="s">
-        <v>450</v>
+        <v>318</v>
       </c>
       <c r="H31" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="L31" t="s">
         <v>44</v>
       </c>
       <c r="AA31" t="s">
-        <v>324</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>223</v>
+        <v>63</v>
       </c>
       <c r="H32" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="L32" t="s">
         <v>45</v>
       </c>
       <c r="AA32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>417</v>
+      </c>
+      <c r="F33" t="s">
+        <v>450</v>
+      </c>
+      <c r="H33" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA33" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33">
-      <c r="F33" t="s">
-        <v>224</v>
-      </c>
-      <c r="H33" t="s">
-        <v>282</v>
-      </c>
-      <c r="AA33" t="s">
+    <row r="34">
+      <c r="A34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F34" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA34" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="F34" t="s">
-        <v>469</v>
-      </c>
-      <c r="H34" t="s">
-        <v>508</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>470</v>
+        <v>224</v>
       </c>
       <c r="H35" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="AA35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>419</v>
+        <v>469</v>
       </c>
       <c r="H36" t="s">
-        <v>327</v>
+        <v>508</v>
       </c>
       <c r="AA36" t="s">
-        <v>543</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>64</v>
+        <v>470</v>
       </c>
       <c r="H37" t="s">
-        <v>304</v>
+        <v>257</v>
       </c>
       <c r="AA37" t="s">
-        <v>117</v>
+        <v>543</v>
       </c>
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>65</v>
+        <v>419</v>
       </c>
       <c r="H38" t="s">
-        <v>258</v>
+        <v>327</v>
       </c>
       <c r="AA38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
       <c r="F39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AA39" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40">
       <c r="F40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H40" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AA40" t="s">
-        <v>119</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41">
       <c r="F41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H41" t="s">
-        <v>78</v>
+        <v>305</v>
       </c>
       <c r="AA41" t="s">
-        <v>335</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42">
       <c r="F42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>210</v>
+        <v>264</v>
       </c>
       <c r="AA42" t="s">
-        <v>432</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43">
       <c r="F43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H43" t="s">
-        <v>539</v>
+        <v>654</v>
       </c>
       <c r="AA43" t="s">
-        <v>552</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44">
       <c r="F44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H44" t="s">
-        <v>286</v>
+        <v>78</v>
       </c>
       <c r="AA44" t="s">
-        <v>396</v>
+        <v>552</v>
       </c>
     </row>
     <row r="45">
       <c r="F45" t="s">
+        <v>70</v>
+      </c>
+      <c r="H45" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="F46" t="s">
+        <v>71</v>
+      </c>
+      <c r="H46" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="F47" t="s">
         <v>588</v>
       </c>
-      <c r="H45" t="s">
-        <v>297</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="H46" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA46" t="s">
+      <c r="H47" t="s">
+        <v>286</v>
+      </c>
+      <c r="AA47" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="H47" t="s">
-        <v>340</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="48">
       <c r="H48" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="AA48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49">
       <c r="H49" t="s">
-        <v>209</v>
+        <v>298</v>
       </c>
       <c r="AA49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50">
       <c r="H50" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="AA50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51">
       <c r="H51" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="AA51" t="s">
-        <v>581</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52">
       <c r="H52" t="s">
-        <v>362</v>
+        <v>209</v>
       </c>
       <c r="AA52" t="s">
-        <v>211</v>
+        <v>581</v>
       </c>
     </row>
     <row r="53">
       <c r="H53" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="AA53" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54">
       <c r="H54" t="s">
-        <v>350</v>
+        <v>655</v>
       </c>
       <c r="AA54" t="s">
-        <v>531</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55">
       <c r="H55" t="s">
-        <v>328</v>
+        <v>656</v>
       </c>
       <c r="AA55" t="s">
-        <v>126</v>
+        <v>531</v>
       </c>
     </row>
     <row r="56">
       <c r="H56" t="s">
-        <v>265</v>
+        <v>657</v>
       </c>
       <c r="AA56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57">
       <c r="H57" t="s">
-        <v>289</v>
+        <v>658</v>
       </c>
       <c r="AA57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58">
       <c r="H58" t="s">
-        <v>290</v>
+        <v>336</v>
       </c>
       <c r="AA58" t="s">
-        <v>484</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59">
       <c r="H59" t="s">
-        <v>540</v>
+        <v>362</v>
       </c>
       <c r="AA59" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60">
       <c r="H60" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="AA60" t="s">
-        <v>129</v>
+        <v>466</v>
       </c>
     </row>
     <row r="61">
       <c r="H61" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="AA61" t="s">
-        <v>343</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62">
       <c r="H62" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="AA62" t="s">
-        <v>460</v>
+        <v>343</v>
       </c>
     </row>
     <row r="63">
       <c r="H63" t="s">
-        <v>334</v>
+        <v>289</v>
       </c>
       <c r="AA63" t="s">
-        <v>130</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64">
       <c r="H64" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="AA64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65">
       <c r="H65" t="s">
-        <v>307</v>
+        <v>540</v>
       </c>
       <c r="AA65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66">
       <c r="H66" t="s">
-        <v>363</v>
+        <v>291</v>
       </c>
       <c r="AA66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67">
       <c r="H67" t="s">
-        <v>364</v>
+        <v>659</v>
       </c>
       <c r="AA67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68">
       <c r="H68" t="s">
-        <v>342</v>
+        <v>660</v>
       </c>
       <c r="AA68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69">
       <c r="H69" t="s">
-        <v>310</v>
+        <v>661</v>
       </c>
       <c r="AA69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70">
       <c r="H70" t="s">
-        <v>266</v>
+        <v>309</v>
       </c>
       <c r="AA70" t="s">
-        <v>441</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71">
       <c r="H71" t="s">
-        <v>527</v>
+        <v>662</v>
       </c>
       <c r="AA71" t="s">
-        <v>474</v>
+        <v>441</v>
       </c>
     </row>
     <row r="72">
       <c r="H72" t="s">
-        <v>311</v>
+        <v>663</v>
       </c>
       <c r="AA72" t="s">
-        <v>212</v>
+        <v>474</v>
       </c>
     </row>
     <row r="73">
       <c r="H73" t="s">
-        <v>413</v>
+        <v>334</v>
       </c>
       <c r="AA73" t="s">
-        <v>392</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74">
       <c r="H74" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="AA74" t="s">
-        <v>445</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75">
       <c r="H75" t="s">
-        <v>414</v>
+        <v>307</v>
       </c>
       <c r="AA75" t="s">
-        <v>137</v>
+        <v>445</v>
       </c>
     </row>
     <row r="76">
       <c r="H76" t="s">
-        <v>259</v>
+        <v>363</v>
       </c>
       <c r="AA76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77">
       <c r="H77" t="s">
-        <v>509</v>
+        <v>364</v>
       </c>
       <c r="AA77" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78">
       <c r="H78" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AA78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79">
       <c r="H79" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="AA79" t="s">
-        <v>628</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80">
       <c r="H80" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="AA80" t="s">
-        <v>195</v>
+        <v>628</v>
       </c>
     </row>
     <row r="81">
       <c r="H81" t="s">
-        <v>288</v>
+        <v>527</v>
       </c>
       <c r="AA81" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82">
       <c r="H82" t="s">
-        <v>420</v>
+        <v>311</v>
       </c>
       <c r="AA82" t="s">
-        <v>455</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83">
       <c r="H83" t="s">
-        <v>329</v>
+        <v>413</v>
       </c>
       <c r="AA83" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>267</v>
+        <v>664</v>
       </c>
       <c r="AA84" t="s">
-        <v>141</v>
+        <v>468</v>
       </c>
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>278</v>
+        <v>665</v>
       </c>
       <c r="AA85" t="s">
-        <v>142</v>
+        <v>673</v>
       </c>
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="AA86" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>273</v>
+        <v>509</v>
       </c>
       <c r="AA87" t="s">
-        <v>496</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>528</v>
+        <v>341</v>
       </c>
       <c r="AA88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="AA89" t="s">
-        <v>145</v>
+        <v>496</v>
       </c>
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>285</v>
+        <v>666</v>
       </c>
       <c r="AA90" t="s">
-        <v>197</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>269</v>
+        <v>667</v>
       </c>
       <c r="AA91" t="s">
-        <v>485</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="AA92" t="s">
-        <v>560</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>302</v>
+        <v>420</v>
       </c>
       <c r="AA93" t="s">
-        <v>198</v>
+        <v>485</v>
       </c>
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="AA94" t="s">
-        <v>454</v>
+        <v>560</v>
       </c>
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="AA95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>337</v>
+        <v>278</v>
       </c>
       <c r="AA96" t="s">
-        <v>200</v>
+        <v>454</v>
       </c>
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="AA97" t="s">
-        <v>546</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98">
       <c r="H98" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA98" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="H99" t="s">
+        <v>528</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="H100" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="H101" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="H102" t="s">
+        <v>668</v>
+      </c>
+      <c r="AA102" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="H103" t="s">
+        <v>669</v>
+      </c>
+      <c r="AA103" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="H104" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="H105" t="s">
+        <v>270</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="H106" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="H107" t="s">
+        <v>308</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="H108" t="s">
+        <v>292</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="H109" t="s">
+        <v>337</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="H110" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="H111" t="s">
         <v>275</v>
       </c>
-      <c r="AA98" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="AA99" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="AA100" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="AA101" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="AA102" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="AA103" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="AA104" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="AA105" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="AA106" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="AA107" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="AA108" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="AA109" t="s">
+      <c r="AA111" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="AA110" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="AA111" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="112">
       <c r="AA112" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113">
       <c r="AA113" t="s">
-        <v>507</v>
+        <v>563</v>
       </c>
     </row>
     <row r="114">
       <c r="AA114" t="s">
-        <v>629</v>
+        <v>206</v>
       </c>
     </row>
     <row r="115">
       <c r="AA115" t="s">
-        <v>630</v>
+        <v>507</v>
       </c>
     </row>
     <row r="116">
       <c r="AA116" t="s">
-        <v>510</v>
+        <v>629</v>
       </c>
     </row>
     <row r="117">
       <c r="AA117" t="s">
-        <v>147</v>
+        <v>630</v>
       </c>
     </row>
     <row r="118">
       <c r="AA118" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="119">
       <c r="AA119" t="s">
-        <v>376</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120">
       <c r="AA120" t="s">
-        <v>148</v>
+        <v>511</v>
       </c>
     </row>
     <row r="121">
       <c r="AA121" t="s">
-        <v>149</v>
+        <v>376</v>
       </c>
     </row>
     <row r="122">
       <c r="AA122" t="s">
-        <v>564</v>
+        <v>148</v>
       </c>
     </row>
     <row r="123">
       <c r="AA123" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124">
       <c r="AA124" t="s">
-        <v>151</v>
+        <v>564</v>
       </c>
     </row>
     <row r="125">
       <c r="AA125" t="s">
-        <v>565</v>
+        <v>150</v>
       </c>
     </row>
     <row r="126">
       <c r="AA126" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="127">
       <c r="AA127" t="s">
-        <v>153</v>
+        <v>565</v>
       </c>
     </row>
     <row r="128">
       <c r="AA128" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129">
       <c r="AA129" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130">
       <c r="AA130" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131">
       <c r="AA131" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132">
       <c r="AA132" t="s">
-        <v>566</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133">
       <c r="AA133" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134">
       <c r="AA134" t="s">
-        <v>159</v>
+        <v>566</v>
       </c>
     </row>
     <row r="135">
       <c r="AA135" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="136">
       <c r="AA136" t="s">
-        <v>582</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137">
       <c r="AA137" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="138">
       <c r="AA138" t="s">
-        <v>544</v>
+        <v>582</v>
       </c>
     </row>
     <row r="139">
       <c r="AA139" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="140">
       <c r="AA140" t="s">
-        <v>163</v>
+        <v>544</v>
       </c>
     </row>
     <row r="141">
       <c r="AA141" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142">
       <c r="AA142" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143">
       <c r="AA143" t="s">
-        <v>631</v>
+        <v>164</v>
       </c>
     </row>
     <row r="144">
       <c r="AA144" t="s">
-        <v>567</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145">
       <c r="AA145" t="s">
-        <v>166</v>
+        <v>631</v>
       </c>
     </row>
     <row r="146">
       <c r="AA146" t="s">
-        <v>167</v>
+        <v>567</v>
       </c>
     </row>
     <row r="147">
       <c r="AA147" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148">
       <c r="AA148" t="s">
-        <v>632</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149">
       <c r="AA149" t="s">
-        <v>633</v>
+        <v>168</v>
       </c>
     </row>
     <row r="150">
       <c r="AA150" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="151">
       <c r="AA151" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="AA152" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="AA153" t="s">
         <v>635</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[io commands] - [assertFileContent(file,match,asLines)]: **NEW** command to automate the assertion of file content.
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt.xlsx
@@ -25,42 +25,45 @@
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
     <definedName name="base">'#system'!$F$2:$F$47</definedName>
-    <definedName name="csv">'#system'!$G$2:$G$6</definedName>
+    <definedName name="csv">'#system'!$H$2:$H$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$111</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$18</definedName>
-    <definedName name="external">'#system'!$J$2:$J$7</definedName>
-    <definedName name="image">'#system'!$K$2:$K$8</definedName>
-    <definedName name="io">'#system'!$L$2:$L$32</definedName>
-    <definedName name="jms">'#system'!$M$2:$M$4</definedName>
-    <definedName name="json">'#system'!$N$2:$N$18</definedName>
-    <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
-    <definedName name="macro">'#system'!$P$2:$P$4</definedName>
-    <definedName name="mail">'#system'!$Q$2:$Q$5</definedName>
+    <definedName name="desktop">'#system'!$I$2:$I$113</definedName>
+    <definedName name="excel">'#system'!$J$2:$J$18</definedName>
+    <definedName name="external">'#system'!$K$2:$K$7</definedName>
+    <definedName name="image">'#system'!$L$2:$L$8</definedName>
+    <definedName name="io">'#system'!$M$2:$M$33</definedName>
+    <definedName name="jms">'#system'!$O$2:$O$4</definedName>
+    <definedName name="json">'#system'!$P$2:$P$19</definedName>
+    <definedName name="localdb">'#system'!$Q$2:$Q$13</definedName>
+    <definedName name="macro">'#system'!$R$2:$R$4</definedName>
+    <definedName name="mail">'#system'!$S$2:$S$5</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$21</definedName>
-    <definedName name="rdbms">'#system'!$T$2:$T$9</definedName>
-    <definedName name="redis">'#system'!$U$2:$U$10</definedName>
-    <definedName name="sms">'#system'!$V$2:$V$2</definedName>
-    <definedName name="sound">'#system'!$W$2:$W$5</definedName>
-    <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
-    <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
-    <definedName name="step.inTime">'#system'!$Z$2:$Z$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$34</definedName>
+    <definedName name="number">'#system'!$U$2:$U$16</definedName>
+    <definedName name="pdf">'#system'!$V$2:$V$21</definedName>
+    <definedName name="rdbms">'#system'!$W$2:$W$9</definedName>
+    <definedName name="redis">'#system'!$X$2:$X$10</definedName>
+    <definedName name="sms">'#system'!$Y$2:$Y$2</definedName>
+    <definedName name="sound">'#system'!$Z$2:$Z$5</definedName>
+    <definedName name="ssh">'#system'!$AA$2:$AA$9</definedName>
+    <definedName name="step">'#system'!$AB$2:$AB$4</definedName>
+    <definedName name="step.inTime">'#system'!$AC$2:$AC$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$38</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
-    <definedName name="tn.5250">'#system'!$AA$2:$AA$38</definedName>
-    <definedName name="web">'#system'!$AA$2:$AA$153</definedName>
-    <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
-    <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
-    <definedName name="ws">'#system'!$AF$2:$AF$17</definedName>
-    <definedName name="ws.async">'#system'!$AG$2:$AG$8</definedName>
-    <definedName name="xml">'#system'!$AH$2:$AH$27</definedName>
-    <definedName name="webmail">'#system'!$AD$2:$AD$4</definedName>
-    <definedName name="word">'#system'!$AE$2:$AE$9</definedName>
+    <definedName name="tn.5250">'#system'!$AD$2:$AD$44</definedName>
+    <definedName name="web">'#system'!$AE$2:$AE$160</definedName>
+    <definedName name="webalert">'#system'!$AF$2:$AF$8</definedName>
+    <definedName name="webcookie">'#system'!$AG$2:$AG$10</definedName>
+    <definedName name="ws">'#system'!$AJ$2:$AJ$20</definedName>
+    <definedName name="ws.async">'#system'!$AK$2:$AK$8</definedName>
+    <definedName name="xml">'#system'!$AL$2:$AL$27</definedName>
+    <definedName name="webmail">'#system'!$AH$2:$AH$6</definedName>
+    <definedName name="word">'#system'!$AI$2:$AI$9</definedName>
+    <definedName name="browserstack">'#system'!$G$2:$G$7</definedName>
+    <definedName name="javaui">'#system'!$N$2:$N$16</definedName>
+    <definedName name="mobile">'#system'!$T$2:$T$51</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -75,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6255" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7036" uniqueCount="771">
   <si>
     <t>description</t>
   </si>
@@ -2130,6 +2133,264 @@
   </si>
   <si>
     <t>removeProtection(file)</t>
+  </si>
+  <si>
+    <t>browserstack</t>
+  </si>
+  <si>
+    <t>javaui</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>deleteApp(profile,appId,resultVar)</t>
+  </si>
+  <si>
+    <t>listBrowsers(profile,resultVar)</t>
+  </si>
+  <si>
+    <t>listDevices(profile,resultVar)</t>
+  </si>
+  <si>
+    <t>saveUploadApps(profile,customId,resultVar)</t>
+  </si>
+  <si>
+    <t>updateSessionStatus(profile,status,reason,resultVar)</t>
+  </si>
+  <si>
+    <t>uploadApp(profile,app,customId,resultVar)</t>
+  </si>
+  <si>
+    <t>focusFirstTableRow()</t>
+  </si>
+  <si>
+    <t>focusLastTableRow()</t>
+  </si>
+  <si>
+    <t>assertFileContent(file,match,asLines)</t>
+  </si>
+  <si>
+    <t>assertEditable(name)</t>
+  </si>
+  <si>
+    <t>assertPresence(name)</t>
+  </si>
+  <si>
+    <t>assertText(name,text)</t>
+  </si>
+  <si>
+    <t>clickMenu(menus)</t>
+  </si>
+  <si>
+    <t>startApp(profile)</t>
+  </si>
+  <si>
+    <t>startLocalAgent$nexial_core(portNumber)</t>
+  </si>
+  <si>
+    <t>startLocalAgent(port)</t>
+  </si>
+  <si>
+    <t>stopApp(profile)</t>
+  </si>
+  <si>
+    <t>stopLocalAgent$nexial_core(portNumber)</t>
+  </si>
+  <si>
+    <t>stopLocalAgent(port)</t>
+  </si>
+  <si>
+    <t>typeText(name,text)</t>
+  </si>
+  <si>
+    <t>waitForWindowTitle(title)</t>
+  </si>
+  <si>
+    <t>sanitize(var,json)</t>
+  </si>
+  <si>
+    <t>assertAlertPresent(text)</t>
+  </si>
+  <si>
+    <t>assertAttribute(locator,attribute,text)</t>
+  </si>
+  <si>
+    <t>assertCount(locator,count)</t>
+  </si>
+  <si>
+    <t>assertElementNotVisible(locator)</t>
+  </si>
+  <si>
+    <t>assertElementVisible(locator)</t>
+  </si>
+  <si>
+    <t>assertLocked()</t>
+  </si>
+  <si>
+    <t>assertTextPresent(locator,text)</t>
+  </si>
+  <si>
+    <t>back()</t>
+  </si>
+  <si>
+    <t>clearAlert(option)</t>
+  </si>
+  <si>
+    <t>clearNotification()</t>
+  </si>
+  <si>
+    <t>clickByDisplayText(text)</t>
+  </si>
+  <si>
+    <t>clickUntilNotFound(locator,waitMs,max)</t>
+  </si>
+  <si>
+    <t>closeApp()</t>
+  </si>
+  <si>
+    <t>copyToLocal(file,folder)</t>
+  </si>
+  <si>
+    <t>doubleClick(locator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>forward()</t>
+  </si>
+  <si>
+    <t>hideKeyboard()</t>
+  </si>
+  <si>
+    <t>home()</t>
+  </si>
+  <si>
+    <t>launchApp(app)</t>
+  </si>
+  <si>
+    <t>lock()</t>
+  </si>
+  <si>
+    <t>longClick(locator,waitMs)</t>
+  </si>
+  <si>
+    <t>orientation(mode)</t>
+  </si>
+  <si>
+    <t>postScreenshot$nexial_core(target,locator)</t>
+  </si>
+  <si>
+    <t>recentApps()</t>
+  </si>
+  <si>
+    <t>saveAlertText(var)</t>
+  </si>
+  <si>
+    <t>saveAttributes(var,locator,attribute)</t>
+  </si>
+  <si>
+    <t>saveLockStatus(var)</t>
+  </si>
+  <si>
+    <t>scroll(locator,direction)</t>
+  </si>
+  <si>
+    <t>scrollUntilFound(scrollTarget,direction,searchFor,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>select(locator,item)</t>
+  </si>
+  <si>
+    <t>selectLocalFile(device,folder,filename)</t>
+  </si>
+  <si>
+    <t>sendSms(phone,message)</t>
+  </si>
+  <si>
+    <t>shake()</t>
+  </si>
+  <si>
+    <t>shutdown(profile)</t>
+  </si>
+  <si>
+    <t>slide(start,end)</t>
+  </si>
+  <si>
+    <t>type(locator,text)</t>
+  </si>
+  <si>
+    <t>unlock()</t>
+  </si>
+  <si>
+    <t>use(profile)</t>
+  </si>
+  <si>
+    <t>zoom(start1,end1,start2,end2)</t>
+  </si>
+  <si>
+    <t>compare$nexial_core(expects,actual,expectMatch,messagePrefix)</t>
+  </si>
+  <si>
+    <t>typeOnMatchedColumns(matches,keystrokes)</t>
+  </si>
+  <si>
+    <t>waitUntilMessagePresent(message,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>waitUntilProcessed(maxWaitMs)</t>
+  </si>
+  <si>
+    <t>waitUntilTextPresent(text,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>waitUntilTitlePresent(title,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>assertElementNotPresent(locator,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>assertElementsEnabled(prefix)</t>
+  </si>
+  <si>
+    <t>assertElementsVisible(prefix)</t>
+  </si>
+  <si>
+    <t>assertSelectOptionsAbsent(locator,options)</t>
+  </si>
+  <si>
+    <t>assertSelectOptionsPresent(locator,options)</t>
+  </si>
+  <si>
+    <t>clickIfPresent(locator)</t>
+  </si>
+  <si>
+    <t>saveCssValue(var,locator,property)</t>
+  </si>
+  <si>
+    <t>selectDropdown(locator,optLocator,optText)</t>
+  </si>
+  <si>
+    <t>toast(message,duration,darkMode)</t>
+  </si>
+  <si>
+    <t>waitForElementTextPresent(locator,text)</t>
+  </si>
+  <si>
+    <t>waitWhileElementNotPresent(locator,waitMs)</t>
+  </si>
+  <si>
+    <t>attachment(profile,id,attachment,saveTo)</t>
+  </si>
+  <si>
+    <t>attachments(profile,id,saveDir)</t>
+  </si>
+  <si>
+    <t>clearHeaders(headers)</t>
+  </si>
+  <si>
+    <t>graphql(url,body,var)</t>
+  </si>
+  <si>
+    <t>oauthProfile(var,profile)</t>
   </si>
 </sst>
 </file>
@@ -2137,7 +2398,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="164" x14ac:knownFonts="1">
+  <fonts count="181" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3177,8 +3438,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="220">
+  <fills count="244">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3195,6 +3563,142 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -4467,7 +4971,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="208">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4957,106 +5461,157 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="168" fontId="129" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="130" fillId="174" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="174" fontId="130" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="131" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="132" fillId="177" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="177" fontId="132" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="133" fillId="180" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="180" fontId="133" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="134" fillId="183" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="183" fontId="134" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="135" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="136" fillId="186" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="186" fontId="136" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="137" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="138" fillId="189" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="189" fontId="138" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="139" fillId="192" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="192" fontId="139" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="140" fillId="180" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="180" fontId="140" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="141" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="142" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="143" fillId="183" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="183" fontId="143" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="144" fillId="195" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="195" fontId="144" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="145" fillId="183" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="183" fontId="145" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="146" fillId="192" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="192" fontId="146" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="147" fillId="198" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="198" fontId="147" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="148" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="149" fillId="201" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="201" fontId="149" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="150" fillId="204" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="204" fontId="150" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="207" fontId="151" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="152" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="153" fillId="210" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="210" fontId="153" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="154" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="155" fillId="213" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="213" fontId="155" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="156" fillId="216" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="216" fontId="156" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="157" fillId="204" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="204" fontId="157" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="158" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="158" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="159" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="160" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="207" fontId="160" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="161" fillId="219" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="219" fontId="161" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="207" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="207" fontId="162" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="163" fillId="216" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="216" fontId="163" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="164" fillId="222" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="166" fillId="225" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="228" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="168" fillId="231" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="170" fillId="234" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="237" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="240" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="228" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="175" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="231" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="243" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="231" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="240" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5471,7 +6026,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI153"/>
+  <dimension ref="A1:AM160"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -5502,87 +6057,99 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>685</v>
+      </c>
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>344</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>686</v>
+      </c>
+      <c r="O1" t="s">
         <v>330</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>512</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>477</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>194</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>687</v>
+      </c>
+      <c r="U1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>237</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>403</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>415</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>416</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>351</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>399</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>573</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
+        <v>583</v>
+      </c>
+      <c r="AE1" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>648</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>649</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>417</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AL1" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5606,87 +6173,99 @@
         <v>58</v>
       </c>
       <c r="G2" t="s">
+        <v>688</v>
+      </c>
+      <c r="H2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>74</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>451</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>637</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>467</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>312</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>390</v>
+      </c>
+      <c r="O2" t="s">
         <v>387</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>421</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>513</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>480</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>642</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
+        <v>710</v>
+      </c>
+      <c r="U2" t="s">
         <v>423</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>251</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>575</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>404</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>427</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>428</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>374</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>400</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>577</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AD2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AE2" t="s">
         <v>96</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AF2" t="s">
         <v>169</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AG2" t="s">
         <v>174</v>
       </c>
-      <c r="AD2" t="s">
-        <v>674</v>
-      </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
+        <v>766</v>
+      </c>
+      <c r="AI2" t="s">
         <v>677</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AJ2" t="s">
         <v>181</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AK2" t="s">
         <v>434</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AL2" t="s">
         <v>491</v>
       </c>
     </row>
@@ -5707,84 +6286,96 @@
         <v>458</v>
       </c>
       <c r="G3" t="s">
+        <v>689</v>
+      </c>
+      <c r="H3" t="s">
         <v>359</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>88</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>49</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>79</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>346</v>
       </c>
-      <c r="L3" t="s">
-        <v>338</v>
-      </c>
       <c r="M3" t="s">
+        <v>696</v>
+      </c>
+      <c r="N3" t="s">
+        <v>697</v>
+      </c>
+      <c r="O3" t="s">
         <v>331</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>86</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>514</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>481</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>643</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
+        <v>711</v>
+      </c>
+      <c r="U3" t="s">
         <v>424</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>238</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>576</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>405</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>429</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>375</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
         <v>401</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
         <v>578</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AD3" t="s">
+        <v>592</v>
+      </c>
+      <c r="AE3" t="s">
         <v>97</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AF3" t="s">
         <v>170</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AG3" t="s">
         <v>175</v>
       </c>
-      <c r="AD3" t="s">
-        <v>675</v>
-      </c>
-      <c r="AE3" t="s">
+      <c r="AH3" t="s">
+        <v>767</v>
+      </c>
+      <c r="AI3" t="s">
         <v>678</v>
       </c>
-      <c r="AF3" t="s">
-        <v>358</v>
-      </c>
-      <c r="AG3" t="s">
+      <c r="AJ3" t="s">
+        <v>768</v>
+      </c>
+      <c r="AK3" t="s">
         <v>182</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AL3" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5802,84 +6393,96 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
+        <v>690</v>
+      </c>
+      <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>390</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>452</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>478</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>347</v>
       </c>
-      <c r="L4" t="s">
-        <v>556</v>
-      </c>
       <c r="M4" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" t="s">
+        <v>391</v>
+      </c>
+      <c r="O4" t="s">
         <v>332</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>25</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>515</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>482</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>422</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
+        <v>712</v>
+      </c>
+      <c r="U4" t="s">
         <v>26</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>239</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>215</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>406</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>430</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" t="s">
         <v>352</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>402</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" t="s">
         <v>579</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AD4" t="s">
+        <v>593</v>
+      </c>
+      <c r="AE4" t="s">
         <v>557</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AF4" t="s">
         <v>171</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AG4" t="s">
         <v>176</v>
       </c>
-      <c r="AD4" t="s">
-        <v>676</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
+        <v>674</v>
+      </c>
+      <c r="AI4" t="s">
         <v>679</v>
       </c>
-      <c r="AF4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
+        <v>358</v>
+      </c>
+      <c r="AK4" t="s">
         <v>435</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AL4" t="s">
         <v>227</v>
       </c>
     </row>
@@ -5897,69 +6500,84 @@
         <v>459</v>
       </c>
       <c r="G5" t="s">
+        <v>691</v>
+      </c>
+      <c r="H5" t="s">
         <v>442</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>545</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>456</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>479</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>348</v>
       </c>
-      <c r="L5" t="s">
-        <v>236</v>
+      <c r="M5" t="s">
+        <v>556</v>
       </c>
       <c r="N5" t="s">
+        <v>698</v>
+      </c>
+      <c r="P5" t="s">
         <v>87</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>524</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>644</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
+        <v>580</v>
+      </c>
+      <c r="U5" t="s">
         <v>29</v>
       </c>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>240</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>216</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>407</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Z5" t="s">
         <v>431</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AA5" t="s">
         <v>353</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AD5" t="s">
+        <v>594</v>
+      </c>
+      <c r="AE5" t="s">
         <v>551</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AF5" t="s">
         <v>172</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AG5" t="s">
         <v>568</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AH5" t="s">
+        <v>675</v>
+      </c>
+      <c r="AI5" t="s">
         <v>680</v>
       </c>
-      <c r="AF5" t="s">
-        <v>183</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AJ5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK5" t="s">
         <v>436</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AL5" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5977,69 +6595,84 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
+        <v>692</v>
+      </c>
+      <c r="H6" t="s">
         <v>503</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>333</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>449</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>526</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>572</v>
       </c>
-      <c r="L6" t="s">
-        <v>463</v>
+      <c r="M6" t="s">
+        <v>236</v>
       </c>
       <c r="N6" t="s">
+        <v>699</v>
+      </c>
+      <c r="P6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>519</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
+        <v>562</v>
+      </c>
+      <c r="U6" t="s">
         <v>30</v>
       </c>
-      <c r="S6" t="s">
+      <c r="V6" t="s">
         <v>241</v>
       </c>
-      <c r="T6" t="s">
+      <c r="W6" t="s">
         <v>217</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
         <v>408</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AA6" t="s">
         <v>355</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AD6" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE6" t="s">
         <v>98</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AF6" t="s">
         <v>446</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AG6" t="s">
         <v>177</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AH6" t="s">
+        <v>676</v>
+      </c>
+      <c r="AI6" t="s">
         <v>681</v>
       </c>
-      <c r="AF6" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG6" t="s">
+      <c r="AJ6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AK6" t="s">
         <v>437</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AL6" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>685</v>
       </c>
       <c r="B7" t="s">
         <v>371</v>
@@ -6047,67 +6680,79 @@
       <c r="F7" t="s">
         <v>222</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
+        <v>693</v>
+      </c>
+      <c r="I7" t="s">
         <v>391</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>448</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>555</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>345</v>
       </c>
-      <c r="L7" t="s">
-        <v>638</v>
+      <c r="M7" t="s">
+        <v>463</v>
       </c>
       <c r="N7" t="s">
+        <v>214</v>
+      </c>
+      <c r="P7" t="s">
         <v>312</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>520</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
+        <v>103</v>
+      </c>
+      <c r="U7" t="s">
         <v>32</v>
       </c>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>242</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" t="s">
         <v>218</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" t="s">
         <v>409</v>
       </c>
-      <c r="X7" t="s">
+      <c r="AA7" t="s">
         <v>354</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AD7" t="s">
+        <v>596</v>
+      </c>
+      <c r="AE7" t="s">
         <v>99</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AF7" t="s">
         <v>447</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AG7" t="s">
         <v>178</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AI7" t="s">
         <v>682</v>
       </c>
-      <c r="AF7" t="s">
-        <v>185</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AJ7" t="s">
+        <v>769</v>
+      </c>
+      <c r="AK7" t="s">
         <v>438</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AL7" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>372</v>
@@ -6115,64 +6760,73 @@
       <c r="F8" t="s">
         <v>315</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>360</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>670</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>529</v>
       </c>
-      <c r="L8" t="s">
-        <v>72</v>
+      <c r="M8" t="s">
+        <v>638</v>
       </c>
       <c r="N8" t="s">
+        <v>700</v>
+      </c>
+      <c r="P8" t="s">
         <v>33</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>521</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
+        <v>713</v>
+      </c>
+      <c r="U8" t="s">
         <v>91</v>
       </c>
-      <c r="S8" t="s">
+      <c r="V8" t="s">
         <v>243</v>
       </c>
-      <c r="T8" t="s">
+      <c r="W8" t="s">
         <v>394</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
         <v>410</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AA8" t="s">
         <v>356</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AD8" t="s">
+        <v>597</v>
+      </c>
+      <c r="AE8" t="s">
         <v>100</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AF8" t="s">
         <v>173</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AG8" t="s">
         <v>179</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AI8" t="s">
         <v>683</v>
       </c>
-      <c r="AF8" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AJ8" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK8" t="s">
         <v>439</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AL8" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>373</v>
@@ -6180,1541 +6834,1870 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>361</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>325</v>
       </c>
-      <c r="L9" t="s">
-        <v>16</v>
+      <c r="M9" t="s">
+        <v>72</v>
       </c>
       <c r="N9" t="s">
+        <v>701</v>
+      </c>
+      <c r="P9" t="s">
         <v>34</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>525</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9" t="s">
         <v>92</v>
       </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
         <v>244</v>
       </c>
-      <c r="T9" t="s">
+      <c r="W9" t="s">
         <v>426</v>
       </c>
-      <c r="U9" t="s">
+      <c r="X9" t="s">
         <v>411</v>
       </c>
-      <c r="X9" t="s">
+      <c r="AA9" t="s">
         <v>357</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AD9" t="s">
+        <v>598</v>
+      </c>
+      <c r="AE9" t="s">
         <v>207</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AG9" t="s">
         <v>180</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AI9" t="s">
         <v>684</v>
       </c>
-      <c r="AF9" t="s">
-        <v>187</v>
-      </c>
-      <c r="AH9" t="s">
+      <c r="AJ9" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL9" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
         <v>312</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>303</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>326</v>
       </c>
-      <c r="L10" t="s">
-        <v>504</v>
+      <c r="M10" t="s">
+        <v>16</v>
       </c>
       <c r="N10" t="s">
+        <v>702</v>
+      </c>
+      <c r="P10" t="s">
         <v>35</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>516</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
+        <v>714</v>
+      </c>
+      <c r="U10" t="s">
         <v>425</v>
       </c>
-      <c r="S10" t="s">
+      <c r="V10" t="s">
         <v>245</v>
       </c>
-      <c r="U10" t="s">
+      <c r="X10" t="s">
         <v>412</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AD10" t="s">
+        <v>599</v>
+      </c>
+      <c r="AE10" t="s">
         <v>254</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AG10" t="s">
         <v>569</v>
       </c>
-      <c r="AF10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH10" t="s">
+      <c r="AJ10" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL10" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>344</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
         <v>636</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>349</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>570</v>
       </c>
-      <c r="L11" t="s">
-        <v>80</v>
+      <c r="M11" t="s">
+        <v>504</v>
       </c>
       <c r="N11" t="s">
+        <v>703</v>
+      </c>
+      <c r="P11" t="s">
         <v>472</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>517</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
+        <v>502</v>
+      </c>
+      <c r="U11" t="s">
         <v>93</v>
       </c>
-      <c r="S11" t="s">
+      <c r="V11" t="s">
         <v>590</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AD11" t="s">
+        <v>600</v>
+      </c>
+      <c r="AE11" t="s">
         <v>255</v>
       </c>
-      <c r="AF11" t="s">
-        <v>256</v>
-      </c>
-      <c r="AH11" t="s">
+      <c r="AJ11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL11" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>344</v>
       </c>
       <c r="F12" t="s">
         <v>550</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>271</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>571</v>
       </c>
-      <c r="L12" t="s">
-        <v>37</v>
+      <c r="M12" t="s">
+        <v>80</v>
       </c>
       <c r="N12" t="s">
+        <v>704</v>
+      </c>
+      <c r="P12" t="s">
         <v>530</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>574</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
+        <v>715</v>
+      </c>
+      <c r="U12" t="s">
         <v>40</v>
       </c>
-      <c r="S12" t="s">
+      <c r="V12" t="s">
         <v>246</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AD12" t="s">
+        <v>601</v>
+      </c>
+      <c r="AE12" t="s">
         <v>101</v>
       </c>
-      <c r="AF12" t="s">
-        <v>189</v>
-      </c>
-      <c r="AH12" t="s">
+      <c r="AJ12" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL12" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>330</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
         <v>316</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>260</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>453</v>
       </c>
-      <c r="L13" t="s">
-        <v>505</v>
+      <c r="M13" t="s">
+        <v>37</v>
       </c>
       <c r="N13" t="s">
+        <v>705</v>
+      </c>
+      <c r="P13" t="s">
         <v>444</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>518</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
+        <v>716</v>
+      </c>
+      <c r="U13" t="s">
         <v>94</v>
       </c>
-      <c r="S13" t="s">
+      <c r="V13" t="s">
         <v>645</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AD13" t="s">
+        <v>602</v>
+      </c>
+      <c r="AE13" t="s">
         <v>323</v>
       </c>
-      <c r="AF13" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH13" t="s">
+      <c r="AJ13" t="s">
+        <v>256</v>
+      </c>
+      <c r="AL13" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>686</v>
       </c>
       <c r="F14" t="s">
         <v>338</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>313</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>319</v>
       </c>
-      <c r="L14" t="s">
-        <v>393</v>
+      <c r="M14" t="s">
+        <v>505</v>
       </c>
       <c r="N14" t="s">
+        <v>706</v>
+      </c>
+      <c r="P14" t="s">
         <v>473</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
+        <v>717</v>
+      </c>
+      <c r="U14" t="s">
         <v>95</v>
       </c>
-      <c r="S14" t="s">
+      <c r="V14" t="s">
         <v>247</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AD14" t="s">
+        <v>603</v>
+      </c>
+      <c r="AE14" t="s">
         <v>102</v>
       </c>
-      <c r="AF14" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH14" t="s">
+      <c r="AJ14" t="s">
+        <v>770</v>
+      </c>
+      <c r="AL14" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>512</v>
+        <v>330</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>261</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>320</v>
       </c>
-      <c r="L15" t="s">
-        <v>17</v>
+      <c r="M15" t="s">
+        <v>393</v>
       </c>
       <c r="N15" t="s">
-        <v>38</v>
-      </c>
-      <c r="R15" t="s">
+        <v>707</v>
+      </c>
+      <c r="P15" t="s">
+        <v>709</v>
+      </c>
+      <c r="T15" t="s">
+        <v>718</v>
+      </c>
+      <c r="U15" t="s">
         <v>500</v>
       </c>
-      <c r="S15" t="s">
+      <c r="V15" t="s">
         <v>561</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AD15" t="s">
+        <v>604</v>
+      </c>
+      <c r="AE15" t="s">
         <v>580</v>
       </c>
-      <c r="AF15" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH15" t="s">
+      <c r="AJ15" t="s">
+        <v>189</v>
+      </c>
+      <c r="AL15" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>477</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>262</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>321</v>
       </c>
-      <c r="L16" t="s">
-        <v>41</v>
+      <c r="M16" t="s">
+        <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>541</v>
-      </c>
-      <c r="R16" t="s">
+        <v>708</v>
+      </c>
+      <c r="P16" t="s">
+        <v>38</v>
+      </c>
+      <c r="T16" t="s">
+        <v>719</v>
+      </c>
+      <c r="U16" t="s">
         <v>501</v>
       </c>
-      <c r="S16" t="s">
+      <c r="V16" t="s">
         <v>252</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AD16" t="s">
+        <v>605</v>
+      </c>
+      <c r="AE16" t="s">
         <v>562</v>
       </c>
-      <c r="AF16" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH16" t="s">
+      <c r="AJ16" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL16" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>512</v>
       </c>
       <c r="F17" t="s">
         <v>388</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>314</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>322</v>
       </c>
-      <c r="L17" t="s">
-        <v>506</v>
-      </c>
-      <c r="N17" t="s">
-        <v>39</v>
-      </c>
-      <c r="S17" t="s">
+      <c r="M17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" t="s">
+        <v>541</v>
+      </c>
+      <c r="T17" t="s">
+        <v>77</v>
+      </c>
+      <c r="V17" t="s">
         <v>248</v>
       </c>
-      <c r="AA17" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>464</v>
-      </c>
-      <c r="AH17" t="s">
+      <c r="AD17" t="s">
+        <v>606</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>755</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL17" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>477</v>
       </c>
       <c r="F18" t="s">
         <v>389</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>89</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>671</v>
       </c>
-      <c r="L18" t="s">
-        <v>81</v>
-      </c>
-      <c r="N18" t="s">
-        <v>42</v>
-      </c>
-      <c r="S18" t="s">
+      <c r="M18" t="s">
+        <v>506</v>
+      </c>
+      <c r="P18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" t="s">
+        <v>720</v>
+      </c>
+      <c r="V18" t="s">
         <v>249</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AD18" t="s">
+        <v>607</v>
+      </c>
+      <c r="AE18" t="s">
         <v>75</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AJ18" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL18" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="F19" t="s">
         <v>650</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>90</v>
       </c>
-      <c r="L19" t="s">
-        <v>82</v>
-      </c>
-      <c r="S19" t="s">
+      <c r="M19" t="s">
+        <v>81</v>
+      </c>
+      <c r="P19" t="s">
+        <v>42</v>
+      </c>
+      <c r="T19" t="s">
+        <v>721</v>
+      </c>
+      <c r="V19" t="s">
         <v>646</v>
       </c>
-      <c r="AA19" t="s">
-        <v>502</v>
-      </c>
-      <c r="AH19" t="s">
+      <c r="AD19" t="s">
+        <v>608</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>756</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL19" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>687</v>
       </c>
       <c r="F20" t="s">
         <v>651</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>293</v>
       </c>
-      <c r="L20" t="s">
-        <v>457</v>
-      </c>
-      <c r="S20" t="s">
+      <c r="M20" t="s">
+        <v>82</v>
+      </c>
+      <c r="T20" t="s">
+        <v>722</v>
+      </c>
+      <c r="V20" t="s">
         <v>250</v>
       </c>
-      <c r="AA20" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH20" t="s">
+      <c r="AD20" t="s">
+        <v>609</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>502</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>464</v>
+      </c>
+      <c r="AL20" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>403</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
         <v>418</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>294</v>
       </c>
-      <c r="L21" t="s">
-        <v>83</v>
-      </c>
-      <c r="S21" t="s">
+      <c r="M21" t="s">
+        <v>457</v>
+      </c>
+      <c r="T21" t="s">
+        <v>723</v>
+      </c>
+      <c r="V21" t="s">
         <v>647</v>
       </c>
-      <c r="AA21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH21" t="s">
+      <c r="AD21" t="s">
+        <v>610</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>757</v>
+      </c>
+      <c r="AL21" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>415</v>
+        <v>237</v>
       </c>
       <c r="F22" t="s">
         <v>584</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>295</v>
       </c>
-      <c r="L22" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH22" t="s">
+      <c r="M22" t="s">
+        <v>83</v>
+      </c>
+      <c r="T22" t="s">
+        <v>724</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL22" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>416</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
         <v>585</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>296</v>
       </c>
-      <c r="L23" t="s">
-        <v>554</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH23" t="s">
+      <c r="M23" t="s">
+        <v>84</v>
+      </c>
+      <c r="T23" t="s">
+        <v>725</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>749</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL23" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>351</v>
+        <v>403</v>
       </c>
       <c r="F24" t="s">
         <v>586</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>287</v>
       </c>
-      <c r="L24" t="s">
-        <v>471</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>483</v>
-      </c>
-      <c r="AH24" t="s">
+      <c r="M24" t="s">
+        <v>554</v>
+      </c>
+      <c r="T24" t="s">
+        <v>726</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>612</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL24" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>399</v>
+        <v>415</v>
       </c>
       <c r="F25" t="s">
         <v>60</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>276</v>
       </c>
-      <c r="L25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH25" t="s">
+      <c r="M25" t="s">
+        <v>471</v>
+      </c>
+      <c r="T25" t="s">
+        <v>727</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>613</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL25" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>573</v>
+        <v>416</v>
       </c>
       <c r="F26" t="s">
         <v>61</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>652</v>
       </c>
-      <c r="L26" t="s">
-        <v>395</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>672</v>
-      </c>
-      <c r="AH26" t="s">
+      <c r="M26" t="s">
+        <v>43</v>
+      </c>
+      <c r="T26" t="s">
+        <v>728</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>614</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>483</v>
+      </c>
+      <c r="AL26" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>351</v>
       </c>
       <c r="F27" t="s">
         <v>253</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>653</v>
       </c>
-      <c r="L27" t="s">
-        <v>589</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>542</v>
-      </c>
-      <c r="AH27" t="s">
+      <c r="M27" t="s">
+        <v>395</v>
+      </c>
+      <c r="T27" t="s">
+        <v>729</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>615</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AL27" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>399</v>
       </c>
       <c r="F28" t="s">
         <v>587</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>76</v>
       </c>
-      <c r="L28" t="s">
-        <v>523</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>109</v>
+      <c r="M28" t="s">
+        <v>589</v>
+      </c>
+      <c r="T28" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>616</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>573</v>
       </c>
       <c r="F29" t="s">
         <v>538</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>279</v>
       </c>
-      <c r="L29" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>110</v>
+      <c r="M29" t="s">
+        <v>523</v>
+      </c>
+      <c r="T29" t="s">
+        <v>731</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>617</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>648</v>
+        <v>583</v>
       </c>
       <c r="F30" t="s">
         <v>62</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>263</v>
       </c>
-      <c r="L30" t="s">
-        <v>443</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>111</v>
+      <c r="M30" t="s">
+        <v>85</v>
+      </c>
+      <c r="T30" t="s">
+        <v>732</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>618</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>649</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
         <v>318</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>280</v>
       </c>
-      <c r="L31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>112</v>
+      <c r="M31" t="s">
+        <v>443</v>
+      </c>
+      <c r="T31" t="s">
+        <v>733</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>619</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F32" t="s">
         <v>63</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>281</v>
       </c>
-      <c r="L32" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>324</v>
+      <c r="M32" t="s">
+        <v>44</v>
+      </c>
+      <c r="T32" t="s">
+        <v>734</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>620</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>417</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
         <v>450</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>214</v>
       </c>
-      <c r="AA33" t="s">
-        <v>113</v>
+      <c r="M33" t="s">
+        <v>45</v>
+      </c>
+      <c r="T33" t="s">
+        <v>735</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>621</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>648</v>
       </c>
       <c r="F34" t="s">
         <v>223</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>272</v>
       </c>
-      <c r="AA34" t="s">
-        <v>114</v>
+      <c r="T34" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>622</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="s">
+        <v>649</v>
+      </c>
       <c r="F35" t="s">
         <v>224</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>282</v>
       </c>
-      <c r="AA35" t="s">
-        <v>115</v>
+      <c r="T35" t="s">
+        <v>736</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>623</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
       <c r="F36" t="s">
         <v>469</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>508</v>
       </c>
-      <c r="AA36" t="s">
-        <v>116</v>
+      <c r="T36" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>624</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="37">
+      <c r="A37" t="s">
+        <v>417</v>
+      </c>
       <c r="F37" t="s">
         <v>470</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>257</v>
       </c>
-      <c r="AA37" t="s">
-        <v>543</v>
+      <c r="T37" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>625</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="s">
+        <v>225</v>
+      </c>
       <c r="F38" t="s">
         <v>419</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>327</v>
       </c>
-      <c r="AA38" t="s">
-        <v>117</v>
+      <c r="T38" t="s">
+        <v>553</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>750</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="39">
       <c r="F39" t="s">
         <v>64</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>304</v>
       </c>
-      <c r="AA39" t="s">
-        <v>118</v>
+      <c r="T39" t="s">
+        <v>737</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>626</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="40">
       <c r="F40" t="s">
         <v>65</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>258</v>
       </c>
-      <c r="AA40" t="s">
-        <v>208</v>
+      <c r="T40" t="s">
+        <v>738</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>627</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="41">
       <c r="F41" t="s">
         <v>66</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>305</v>
       </c>
-      <c r="AA41" t="s">
-        <v>119</v>
+      <c r="T41" t="s">
+        <v>739</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>751</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="42">
       <c r="F42" t="s">
         <v>67</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>264</v>
       </c>
-      <c r="AA42" t="s">
-        <v>335</v>
+      <c r="T42" t="s">
+        <v>740</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>752</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="43">
       <c r="F43" t="s">
         <v>68</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>654</v>
       </c>
-      <c r="AA43" t="s">
-        <v>432</v>
+      <c r="T43" t="s">
+        <v>741</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>753</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44">
       <c r="F44" t="s">
         <v>69</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>78</v>
       </c>
-      <c r="AA44" t="s">
-        <v>552</v>
+      <c r="T44" t="s">
+        <v>742</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>754</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="45">
       <c r="F45" t="s">
         <v>70</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>210</v>
       </c>
-      <c r="AA45" t="s">
-        <v>396</v>
+      <c r="T45" t="s">
+        <v>743</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="46">
       <c r="F46" t="s">
         <v>71</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>539</v>
       </c>
-      <c r="AA46" t="s">
-        <v>120</v>
+      <c r="T46" t="s">
+        <v>744</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="47">
       <c r="F47" t="s">
         <v>588</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>286</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="T47" t="s">
+        <v>745</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="I48" t="s">
+        <v>297</v>
+      </c>
+      <c r="T48" t="s">
+        <v>746</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="I49" t="s">
+        <v>298</v>
+      </c>
+      <c r="T49" t="s">
+        <v>747</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="I50" t="s">
+        <v>340</v>
+      </c>
+      <c r="T50" t="s">
+        <v>631</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="I51" t="s">
+        <v>339</v>
+      </c>
+      <c r="T51" t="s">
+        <v>748</v>
+      </c>
+      <c r="AE51" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48">
-      <c r="H48" t="s">
-        <v>297</v>
-      </c>
-      <c r="AA48" t="s">
+    <row r="52">
+      <c r="I52" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE52" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49">
-      <c r="H49" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA49" t="s">
+    <row r="53">
+      <c r="I53" t="s">
+        <v>317</v>
+      </c>
+      <c r="AE53" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50">
-      <c r="H50" t="s">
-        <v>340</v>
-      </c>
-      <c r="AA50" t="s">
+    <row r="54">
+      <c r="I54" t="s">
+        <v>655</v>
+      </c>
+      <c r="AE54" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51">
-      <c r="H51" t="s">
-        <v>339</v>
-      </c>
-      <c r="AA51" t="s">
+    <row r="55">
+      <c r="I55" t="s">
+        <v>656</v>
+      </c>
+      <c r="AE55" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52">
-      <c r="H52" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA52" t="s">
+    <row r="56">
+      <c r="I56" t="s">
+        <v>657</v>
+      </c>
+      <c r="AE56" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="53">
-      <c r="H53" t="s">
-        <v>317</v>
-      </c>
-      <c r="AA53" t="s">
+    <row r="57">
+      <c r="I57" t="s">
+        <v>658</v>
+      </c>
+      <c r="AE57" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="54">
-      <c r="H54" t="s">
-        <v>655</v>
-      </c>
-      <c r="AA54" t="s">
+    <row r="58">
+      <c r="I58" t="s">
+        <v>336</v>
+      </c>
+      <c r="AE58" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55">
-      <c r="H55" t="s">
-        <v>656</v>
-      </c>
-      <c r="AA55" t="s">
+    <row r="59">
+      <c r="I59" t="s">
+        <v>362</v>
+      </c>
+      <c r="AE59" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="56">
-      <c r="H56" t="s">
-        <v>657</v>
-      </c>
-      <c r="AA56" t="s">
+    <row r="60">
+      <c r="I60" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE60" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="57">
-      <c r="H57" t="s">
-        <v>658</v>
-      </c>
-      <c r="AA57" t="s">
+    <row r="61">
+      <c r="I61" t="s">
+        <v>694</v>
+      </c>
+      <c r="AE61" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="58">
-      <c r="H58" t="s">
-        <v>336</v>
-      </c>
-      <c r="AA58" t="s">
+    <row r="62">
+      <c r="I62" t="s">
+        <v>695</v>
+      </c>
+      <c r="AE62" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="59">
-      <c r="H59" t="s">
-        <v>362</v>
-      </c>
-      <c r="AA59" t="s">
+    <row r="63">
+      <c r="I63" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="I64" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE64" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="60">
-      <c r="H60" t="s">
-        <v>299</v>
-      </c>
-      <c r="AA60" t="s">
+    <row r="65">
+      <c r="I65" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE65" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="61">
-      <c r="H61" t="s">
-        <v>328</v>
-      </c>
-      <c r="AA61" t="s">
+    <row r="66">
+      <c r="I66" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE66" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62">
-      <c r="H62" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA62" t="s">
+    <row r="67">
+      <c r="I67" t="s">
+        <v>540</v>
+      </c>
+      <c r="AE67" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="63">
-      <c r="H63" t="s">
-        <v>289</v>
-      </c>
-      <c r="AA63" t="s">
+    <row r="68">
+      <c r="I68" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE68" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="64">
-      <c r="H64" t="s">
-        <v>290</v>
-      </c>
-      <c r="AA64" t="s">
+    <row r="69">
+      <c r="I69" t="s">
+        <v>659</v>
+      </c>
+      <c r="AE69" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65">
-      <c r="H65" t="s">
-        <v>540</v>
-      </c>
-      <c r="AA65" t="s">
+    <row r="70">
+      <c r="I70" t="s">
+        <v>660</v>
+      </c>
+      <c r="AE70" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="66">
-      <c r="H66" t="s">
-        <v>291</v>
-      </c>
-      <c r="AA66" t="s">
+    <row r="71">
+      <c r="I71" t="s">
+        <v>661</v>
+      </c>
+      <c r="AE71" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="67">
-      <c r="H67" t="s">
-        <v>659</v>
-      </c>
-      <c r="AA67" t="s">
+    <row r="72">
+      <c r="I72" t="s">
+        <v>309</v>
+      </c>
+      <c r="AE72" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68">
-      <c r="H68" t="s">
-        <v>660</v>
-      </c>
-      <c r="AA68" t="s">
+    <row r="73">
+      <c r="I73" t="s">
+        <v>662</v>
+      </c>
+      <c r="AE73" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69">
-      <c r="H69" t="s">
-        <v>661</v>
-      </c>
-      <c r="AA69" t="s">
+    <row r="74">
+      <c r="I74" t="s">
+        <v>663</v>
+      </c>
+      <c r="AE74" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="70">
-      <c r="H70" t="s">
-        <v>309</v>
-      </c>
-      <c r="AA70" t="s">
+    <row r="75">
+      <c r="I75" t="s">
+        <v>334</v>
+      </c>
+      <c r="AE75" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="71">
-      <c r="H71" t="s">
-        <v>662</v>
-      </c>
-      <c r="AA71" t="s">
+    <row r="76">
+      <c r="I76" t="s">
+        <v>306</v>
+      </c>
+      <c r="AE76" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="72">
-      <c r="H72" t="s">
-        <v>663</v>
-      </c>
-      <c r="AA72" t="s">
+    <row r="77">
+      <c r="I77" t="s">
+        <v>307</v>
+      </c>
+      <c r="AE77" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="73">
-      <c r="H73" t="s">
-        <v>334</v>
-      </c>
-      <c r="AA73" t="s">
+    <row r="78">
+      <c r="I78" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE78" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="74">
-      <c r="H74" t="s">
-        <v>306</v>
-      </c>
-      <c r="AA74" t="s">
+    <row r="79">
+      <c r="I79" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE79" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="75">
-      <c r="H75" t="s">
-        <v>307</v>
-      </c>
-      <c r="AA75" t="s">
+    <row r="80">
+      <c r="I80" t="s">
+        <v>342</v>
+      </c>
+      <c r="AE80" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="76">
-      <c r="H76" t="s">
-        <v>363</v>
-      </c>
-      <c r="AA76" t="s">
+    <row r="81">
+      <c r="I81" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE81" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="77">
-      <c r="H77" t="s">
-        <v>364</v>
-      </c>
-      <c r="AA77" t="s">
+    <row r="82">
+      <c r="I82" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE82" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78">
-      <c r="H78" t="s">
-        <v>342</v>
-      </c>
-      <c r="AA78" t="s">
+    <row r="83">
+      <c r="I83" t="s">
+        <v>527</v>
+      </c>
+      <c r="AE83" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="79">
-      <c r="H79" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA79" t="s">
+    <row r="84">
+      <c r="I84" t="s">
+        <v>311</v>
+      </c>
+      <c r="AE84" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="80">
-      <c r="H80" t="s">
-        <v>266</v>
-      </c>
-      <c r="AA80" t="s">
+    <row r="85">
+      <c r="I85" t="s">
+        <v>413</v>
+      </c>
+      <c r="AE85" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="81">
-      <c r="H81" t="s">
-        <v>527</v>
-      </c>
-      <c r="AA81" t="s">
+    <row r="86">
+      <c r="I86" t="s">
+        <v>664</v>
+      </c>
+      <c r="AE86" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="82">
-      <c r="H82" t="s">
-        <v>311</v>
-      </c>
-      <c r="AA82" t="s">
+    <row r="87">
+      <c r="I87" t="s">
+        <v>665</v>
+      </c>
+      <c r="AE87" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="83">
-      <c r="H83" t="s">
-        <v>413</v>
-      </c>
-      <c r="AA83" t="s">
+    <row r="88">
+      <c r="I88" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE88" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="84">
-      <c r="H84" t="s">
-        <v>664</v>
-      </c>
-      <c r="AA84" t="s">
+    <row r="89">
+      <c r="I89" t="s">
+        <v>509</v>
+      </c>
+      <c r="AE89" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="85">
-      <c r="H85" t="s">
-        <v>665</v>
-      </c>
-      <c r="AA85" t="s">
+    <row r="90">
+      <c r="I90" t="s">
+        <v>341</v>
+      </c>
+      <c r="AE90" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="86">
-      <c r="H86" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA86" t="s">
+    <row r="91">
+      <c r="I91" t="s">
+        <v>277</v>
+      </c>
+      <c r="AE91" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="87">
-      <c r="H87" t="s">
-        <v>509</v>
-      </c>
-      <c r="AA87" t="s">
+    <row r="92">
+      <c r="I92" t="s">
+        <v>666</v>
+      </c>
+      <c r="AE92" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="88">
-      <c r="H88" t="s">
-        <v>341</v>
-      </c>
-      <c r="AA88" t="s">
+    <row r="93">
+      <c r="I93" t="s">
+        <v>667</v>
+      </c>
+      <c r="AE93" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="89">
-      <c r="H89" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA89" t="s">
+    <row r="94">
+      <c r="I94" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE94" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="90">
-      <c r="H90" t="s">
-        <v>666</v>
-      </c>
-      <c r="AA90" t="s">
+    <row r="95">
+      <c r="I95" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE95" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="91">
-      <c r="H91" t="s">
-        <v>667</v>
-      </c>
-      <c r="AA91" t="s">
+    <row r="96">
+      <c r="I96" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE96" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="92">
-      <c r="H92" t="s">
-        <v>288</v>
-      </c>
-      <c r="AA92" t="s">
+    <row r="97">
+      <c r="I97" t="s">
+        <v>267</v>
+      </c>
+      <c r="AE97" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="93">
-      <c r="H93" t="s">
-        <v>420</v>
-      </c>
-      <c r="AA93" t="s">
+    <row r="98">
+      <c r="I98" t="s">
+        <v>278</v>
+      </c>
+      <c r="AE98" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="94">
-      <c r="H94" t="s">
-        <v>329</v>
-      </c>
-      <c r="AA94" t="s">
+    <row r="99">
+      <c r="I99" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE99" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="95">
-      <c r="H95" t="s">
-        <v>267</v>
-      </c>
-      <c r="AA95" t="s">
+    <row r="100">
+      <c r="I100" t="s">
+        <v>273</v>
+      </c>
+      <c r="AE100" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="96">
-      <c r="H96" t="s">
-        <v>278</v>
-      </c>
-      <c r="AA96" t="s">
+    <row r="101">
+      <c r="I101" t="s">
+        <v>528</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="I102" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE102" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="97">
-      <c r="H97" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA97" t="s">
+    <row r="103">
+      <c r="I103" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE103" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="98">
-      <c r="H98" t="s">
-        <v>273</v>
-      </c>
-      <c r="AA98" t="s">
+    <row r="104">
+      <c r="I104" t="s">
+        <v>668</v>
+      </c>
+      <c r="AE104" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="99">
-      <c r="H99" t="s">
-        <v>528</v>
-      </c>
-      <c r="AA99" t="s">
+    <row r="105">
+      <c r="I105" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE105" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="100">
-      <c r="H100" t="s">
-        <v>268</v>
-      </c>
-      <c r="AA100" t="s">
+    <row r="106">
+      <c r="I106" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE106" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="101">
-      <c r="H101" t="s">
-        <v>285</v>
-      </c>
-      <c r="AA101" t="s">
+    <row r="107">
+      <c r="I107" t="s">
+        <v>270</v>
+      </c>
+      <c r="AE107" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="102">
-      <c r="H102" t="s">
-        <v>668</v>
-      </c>
-      <c r="AA102" t="s">
+    <row r="108">
+      <c r="I108" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE108" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="103">
-      <c r="H103" t="s">
-        <v>669</v>
-      </c>
-      <c r="AA103" t="s">
+    <row r="109">
+      <c r="I109" t="s">
+        <v>308</v>
+      </c>
+      <c r="AE109" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="104">
-      <c r="H104" t="s">
-        <v>269</v>
-      </c>
-      <c r="AA104" t="s">
+    <row r="110">
+      <c r="I110" t="s">
+        <v>292</v>
+      </c>
+      <c r="AE110" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="105">
-      <c r="H105" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA105" t="s">
+    <row r="111">
+      <c r="I111" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE111" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="106">
-      <c r="H106" t="s">
-        <v>302</v>
-      </c>
-      <c r="AA106" t="s">
+    <row r="112">
+      <c r="I112" t="s">
+        <v>274</v>
+      </c>
+      <c r="AE112" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="107">
-      <c r="H107" t="s">
-        <v>308</v>
-      </c>
-      <c r="AA107" t="s">
+    <row r="113">
+      <c r="I113" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE113" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="108">
-      <c r="H108" t="s">
-        <v>292</v>
-      </c>
-      <c r="AA108" t="s">
+    <row r="114">
+      <c r="AE114" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="109">
-      <c r="H109" t="s">
-        <v>337</v>
-      </c>
-      <c r="AA109" t="s">
+    <row r="115">
+      <c r="AE115" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="110">
-      <c r="H110" t="s">
-        <v>274</v>
-      </c>
-      <c r="AA110" t="s">
+    <row r="116">
+      <c r="AE116" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="111">
-      <c r="H111" t="s">
-        <v>275</v>
-      </c>
-      <c r="AA111" t="s">
+    <row r="117">
+      <c r="AE117" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="112">
-      <c r="AA112" t="s">
+    <row r="118">
+      <c r="AE118" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="113">
-      <c r="AA113" t="s">
+    <row r="119">
+      <c r="AE119" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="114">
-      <c r="AA114" t="s">
+    <row r="120">
+      <c r="AE120" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="115">
-      <c r="AA115" t="s">
+    <row r="121">
+      <c r="AE121" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="116">
-      <c r="AA116" t="s">
+    <row r="122">
+      <c r="AE122" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="117">
-      <c r="AA117" t="s">
+    <row r="123">
+      <c r="AE123" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="118">
-      <c r="AA118" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="AA119" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="AA120" t="s">
+    <row r="124">
+      <c r="AE124" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="121">
-      <c r="AA121" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="AA122" t="s">
+    <row r="125">
+      <c r="AE125" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="123">
-      <c r="AA123" t="s">
+    <row r="126">
+      <c r="AE126" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="124">
-      <c r="AA124" t="s">
+    <row r="127">
+      <c r="AE127" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="125">
-      <c r="AA125" t="s">
+    <row r="128">
+      <c r="AE128" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="AE129" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="126">
-      <c r="AA126" t="s">
+    <row r="130">
+      <c r="AE130" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="127">
-      <c r="AA127" t="s">
+    <row r="131">
+      <c r="AE131" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="128">
-      <c r="AA128" t="s">
+    <row r="132">
+      <c r="AE132" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="129">
-      <c r="AA129" t="s">
+    <row r="133">
+      <c r="AE133" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="130">
-      <c r="AA130" t="s">
+    <row r="134">
+      <c r="AE134" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="131">
-      <c r="AA131" t="s">
+    <row r="135">
+      <c r="AE135" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="132">
-      <c r="AA132" t="s">
+    <row r="136">
+      <c r="AE136" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="133">
-      <c r="AA133" t="s">
+    <row r="137">
+      <c r="AE137" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="134">
-      <c r="AA134" t="s">
+    <row r="138">
+      <c r="AE138" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="135">
-      <c r="AA135" t="s">
+    <row r="139">
+      <c r="AE139" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="AE140" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="136">
-      <c r="AA136" t="s">
+    <row r="141">
+      <c r="AE141" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="137">
-      <c r="AA137" t="s">
+    <row r="142">
+      <c r="AE142" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="138">
-      <c r="AA138" t="s">
+    <row r="143">
+      <c r="AE143" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="139">
-      <c r="AA139" t="s">
+    <row r="144">
+      <c r="AE144" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="140">
-      <c r="AA140" t="s">
+    <row r="145">
+      <c r="AE145" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="141">
-      <c r="AA141" t="s">
+    <row r="146">
+      <c r="AE146" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="142">
-      <c r="AA142" t="s">
+    <row r="147">
+      <c r="AE147" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="143">
-      <c r="AA143" t="s">
+    <row r="148">
+      <c r="AE148" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="144">
-      <c r="AA144" t="s">
+    <row r="149">
+      <c r="AE149" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="145">
-      <c r="AA145" t="s">
+    <row r="150">
+      <c r="AE150" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="146">
-      <c r="AA146" t="s">
+    <row r="151">
+      <c r="AE151" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="AE152" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="147">
-      <c r="AA147" t="s">
+    <row r="153">
+      <c r="AE153" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="148">
-      <c r="AA148" t="s">
+    <row r="154">
+      <c r="AE154" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="149">
-      <c r="AA149" t="s">
+    <row r="155">
+      <c r="AE155" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="150">
-      <c r="AA150" t="s">
+    <row r="156">
+      <c r="AE156" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="151">
-      <c r="AA151" t="s">
+    <row r="157">
+      <c r="AE157" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="152">
-      <c r="AA152" t="s">
+    <row r="158">
+      <c r="AE158" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="153">
-      <c r="AA153" t="s">
+    <row r="159">
+      <c r="AE159" t="s">
         <v>635</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="AE160" t="s">
+        <v>765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>